<commit_message>
Add: add more expenses for monthly subscriptions (spotify, netflix)
</commit_message>
<xml_diff>
--- a/data/expense_tracker.xlsx
+++ b/data/expense_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\solutions\learning_python\expense_tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21503CDD-D891-4AC9-A529-622461B4D5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A394EEC-3430-42DF-BD06-B89BCDED0A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" xr2:uid="{7A62D1F9-0105-4F41-8BB8-21CA3D721AF6}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="9" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">total!$A$1:$L$1630</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">total!$A$1:$L$1724</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6363" uniqueCount="982">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6429" uniqueCount="986">
   <si>
     <t>expense_type</t>
   </si>
@@ -2986,6 +2986,18 @@
   </si>
   <si>
     <t>cottage cheese 250g</t>
+  </si>
+  <si>
+    <t>spotify</t>
+  </si>
+  <si>
+    <t>spotify subscription</t>
+  </si>
+  <si>
+    <t>netflix subscription</t>
+  </si>
+  <si>
+    <t>netflix</t>
   </si>
 </sst>
 </file>
@@ -3338,11 +3350,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397426C9-9494-4E73-BF9B-2DE40DB1433B}">
-  <dimension ref="A1:L1724"/>
+  <dimension ref="A1:L1746"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1702" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1711" sqref="I1711"/>
+      <pane ySplit="1" topLeftCell="A1728" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J1737" sqref="J1737:J1746"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -66032,23 +66044,23 @@
         <v>0.99</v>
       </c>
       <c r="E1715">
-        <f t="shared" ref="E1715:E1724" si="253">MONTH(A1715)</f>
+        <f t="shared" ref="E1715:E1735" si="253">MONTH(A1715)</f>
         <v>4</v>
       </c>
       <c r="F1715">
-        <f t="shared" ref="F1715:F1724" si="254">YEAR(A1715)</f>
+        <f t="shared" ref="F1715:F1735" si="254">YEAR(A1715)</f>
         <v>2024</v>
       </c>
       <c r="G1715">
-        <f t="shared" ref="G1715:G1724" si="255">WEEKDAY(A1715, 2)</f>
+        <f t="shared" ref="G1715:G1735" si="255">WEEKDAY(A1715, 2)</f>
         <v>6</v>
       </c>
       <c r="H1715" t="str">
-        <f t="shared" ref="H1715:H1724" si="256">CHOOSE(WEEKDAY(A1715, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <f t="shared" ref="H1715:H1735" si="256">CHOOSE(WEEKDAY(A1715, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
         <v>Saturday</v>
       </c>
       <c r="I1715" t="str">
-        <f t="shared" ref="I1715:I1724" si="257">TEXT(A1715, "MMM")</f>
+        <f t="shared" ref="I1715:I1735" si="257">TEXT(A1715, "MMM")</f>
         <v>Apr</v>
       </c>
       <c r="J1715" t="s">
@@ -66418,6 +66430,820 @@
       </c>
       <c r="K1724" t="s">
         <v>730</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1725" s="1">
+        <v>45092</v>
+      </c>
+      <c r="B1725" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1725" t="s">
+        <v>983</v>
+      </c>
+      <c r="D1725">
+        <v>5.99</v>
+      </c>
+      <c r="E1725">
+        <f t="shared" si="253"/>
+        <v>6</v>
+      </c>
+      <c r="F1725">
+        <f t="shared" si="254"/>
+        <v>2023</v>
+      </c>
+      <c r="G1725">
+        <f t="shared" si="255"/>
+        <v>4</v>
+      </c>
+      <c r="H1725" t="str">
+        <f t="shared" si="256"/>
+        <v>Thursday</v>
+      </c>
+      <c r="I1725" t="str">
+        <f t="shared" si="257"/>
+        <v>Jun</v>
+      </c>
+      <c r="J1725" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="1726" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1726" s="1">
+        <v>45122</v>
+      </c>
+      <c r="B1726" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1726" t="s">
+        <v>983</v>
+      </c>
+      <c r="D1726">
+        <v>5.99</v>
+      </c>
+      <c r="E1726">
+        <f t="shared" si="253"/>
+        <v>7</v>
+      </c>
+      <c r="F1726">
+        <f t="shared" si="254"/>
+        <v>2023</v>
+      </c>
+      <c r="G1726">
+        <f t="shared" si="255"/>
+        <v>6</v>
+      </c>
+      <c r="H1726" t="str">
+        <f t="shared" si="256"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1726" t="str">
+        <f t="shared" si="257"/>
+        <v>Jul</v>
+      </c>
+      <c r="J1726" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1727" s="1">
+        <v>45153</v>
+      </c>
+      <c r="B1727" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1727" t="s">
+        <v>983</v>
+      </c>
+      <c r="D1727">
+        <v>5.99</v>
+      </c>
+      <c r="E1727">
+        <f t="shared" si="253"/>
+        <v>8</v>
+      </c>
+      <c r="F1727">
+        <f t="shared" si="254"/>
+        <v>2023</v>
+      </c>
+      <c r="G1727">
+        <f t="shared" si="255"/>
+        <v>2</v>
+      </c>
+      <c r="H1727" t="str">
+        <f t="shared" si="256"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1727" t="str">
+        <f t="shared" si="257"/>
+        <v>Aug</v>
+      </c>
+      <c r="J1727" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1728" s="1">
+        <v>45184</v>
+      </c>
+      <c r="B1728" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1728" t="s">
+        <v>983</v>
+      </c>
+      <c r="D1728">
+        <v>5.99</v>
+      </c>
+      <c r="E1728">
+        <f t="shared" si="253"/>
+        <v>9</v>
+      </c>
+      <c r="F1728">
+        <f t="shared" si="254"/>
+        <v>2023</v>
+      </c>
+      <c r="G1728">
+        <f t="shared" si="255"/>
+        <v>5</v>
+      </c>
+      <c r="H1728" t="str">
+        <f t="shared" si="256"/>
+        <v>Friday</v>
+      </c>
+      <c r="I1728" t="str">
+        <f t="shared" si="257"/>
+        <v>Sep</v>
+      </c>
+      <c r="J1728" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1729" s="1">
+        <v>45214</v>
+      </c>
+      <c r="B1729" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1729" t="s">
+        <v>983</v>
+      </c>
+      <c r="D1729">
+        <v>5.99</v>
+      </c>
+      <c r="E1729">
+        <f t="shared" si="253"/>
+        <v>10</v>
+      </c>
+      <c r="F1729">
+        <f t="shared" si="254"/>
+        <v>2023</v>
+      </c>
+      <c r="G1729">
+        <f t="shared" si="255"/>
+        <v>7</v>
+      </c>
+      <c r="H1729" t="str">
+        <f t="shared" si="256"/>
+        <v>Sunday</v>
+      </c>
+      <c r="I1729" t="str">
+        <f t="shared" si="257"/>
+        <v>Oct</v>
+      </c>
+      <c r="J1729" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1730" s="1">
+        <v>45245</v>
+      </c>
+      <c r="B1730" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1730" t="s">
+        <v>983</v>
+      </c>
+      <c r="D1730">
+        <v>5.99</v>
+      </c>
+      <c r="E1730">
+        <f t="shared" si="253"/>
+        <v>11</v>
+      </c>
+      <c r="F1730">
+        <f t="shared" si="254"/>
+        <v>2023</v>
+      </c>
+      <c r="G1730">
+        <f t="shared" si="255"/>
+        <v>3</v>
+      </c>
+      <c r="H1730" t="str">
+        <f t="shared" si="256"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="I1730" t="str">
+        <f t="shared" si="257"/>
+        <v>Nov</v>
+      </c>
+      <c r="J1730" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1731" s="1">
+        <v>45275</v>
+      </c>
+      <c r="B1731" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1731" t="s">
+        <v>983</v>
+      </c>
+      <c r="D1731">
+        <v>5.99</v>
+      </c>
+      <c r="E1731">
+        <f t="shared" si="253"/>
+        <v>12</v>
+      </c>
+      <c r="F1731">
+        <f t="shared" si="254"/>
+        <v>2023</v>
+      </c>
+      <c r="G1731">
+        <f t="shared" si="255"/>
+        <v>5</v>
+      </c>
+      <c r="H1731" t="str">
+        <f t="shared" si="256"/>
+        <v>Friday</v>
+      </c>
+      <c r="I1731" t="str">
+        <f t="shared" si="257"/>
+        <v>Dec</v>
+      </c>
+      <c r="J1731" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1732" s="1">
+        <v>45306</v>
+      </c>
+      <c r="B1732" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1732" t="s">
+        <v>983</v>
+      </c>
+      <c r="D1732">
+        <v>5.99</v>
+      </c>
+      <c r="E1732">
+        <f t="shared" si="253"/>
+        <v>1</v>
+      </c>
+      <c r="F1732">
+        <f t="shared" si="254"/>
+        <v>2024</v>
+      </c>
+      <c r="G1732">
+        <f t="shared" si="255"/>
+        <v>1</v>
+      </c>
+      <c r="H1732" t="str">
+        <f t="shared" si="256"/>
+        <v>Monday</v>
+      </c>
+      <c r="I1732" t="str">
+        <f t="shared" si="257"/>
+        <v>Jan</v>
+      </c>
+      <c r="J1732" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1733" s="1">
+        <v>45337</v>
+      </c>
+      <c r="B1733" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1733" t="s">
+        <v>983</v>
+      </c>
+      <c r="D1733">
+        <v>5.99</v>
+      </c>
+      <c r="E1733">
+        <f t="shared" si="253"/>
+        <v>2</v>
+      </c>
+      <c r="F1733">
+        <f t="shared" si="254"/>
+        <v>2024</v>
+      </c>
+      <c r="G1733">
+        <f t="shared" si="255"/>
+        <v>4</v>
+      </c>
+      <c r="H1733" t="str">
+        <f t="shared" si="256"/>
+        <v>Thursday</v>
+      </c>
+      <c r="I1733" t="str">
+        <f t="shared" si="257"/>
+        <v>Feb</v>
+      </c>
+      <c r="J1733" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1734" s="1">
+        <v>45366</v>
+      </c>
+      <c r="B1734" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1734" t="s">
+        <v>983</v>
+      </c>
+      <c r="D1734">
+        <v>5.99</v>
+      </c>
+      <c r="E1734">
+        <f t="shared" si="253"/>
+        <v>3</v>
+      </c>
+      <c r="F1734">
+        <f t="shared" si="254"/>
+        <v>2024</v>
+      </c>
+      <c r="G1734">
+        <f t="shared" si="255"/>
+        <v>5</v>
+      </c>
+      <c r="H1734" t="str">
+        <f t="shared" si="256"/>
+        <v>Friday</v>
+      </c>
+      <c r="I1734" t="str">
+        <f t="shared" si="257"/>
+        <v>Mar</v>
+      </c>
+      <c r="J1734" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1735" s="1">
+        <v>45397</v>
+      </c>
+      <c r="B1735" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1735" t="s">
+        <v>983</v>
+      </c>
+      <c r="D1735">
+        <v>5.99</v>
+      </c>
+      <c r="E1735">
+        <f t="shared" si="253"/>
+        <v>4</v>
+      </c>
+      <c r="F1735">
+        <f t="shared" si="254"/>
+        <v>2024</v>
+      </c>
+      <c r="G1735">
+        <f t="shared" si="255"/>
+        <v>1</v>
+      </c>
+      <c r="H1735" t="str">
+        <f t="shared" si="256"/>
+        <v>Monday</v>
+      </c>
+      <c r="I1735" t="str">
+        <f t="shared" si="257"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1735" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1736" s="1">
+        <v>45082</v>
+      </c>
+      <c r="B1736" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1736" t="s">
+        <v>984</v>
+      </c>
+      <c r="D1736">
+        <v>7.99</v>
+      </c>
+      <c r="E1736">
+        <f t="shared" ref="E1736:E1746" si="258">MONTH(A1736)</f>
+        <v>6</v>
+      </c>
+      <c r="F1736">
+        <f t="shared" ref="F1736:F1746" si="259">YEAR(A1736)</f>
+        <v>2023</v>
+      </c>
+      <c r="G1736">
+        <f t="shared" ref="G1736:G1746" si="260">WEEKDAY(A1736, 2)</f>
+        <v>1</v>
+      </c>
+      <c r="H1736" t="str">
+        <f t="shared" ref="H1736:H1746" si="261">CHOOSE(WEEKDAY(A1736, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Monday</v>
+      </c>
+      <c r="I1736" t="str">
+        <f t="shared" ref="I1736:I1746" si="262">TEXT(A1736, "MMM")</f>
+        <v>Jun</v>
+      </c>
+      <c r="J1736" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1737" s="1">
+        <v>45112</v>
+      </c>
+      <c r="B1737" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1737" t="s">
+        <v>984</v>
+      </c>
+      <c r="D1737">
+        <v>7.99</v>
+      </c>
+      <c r="E1737">
+        <f t="shared" si="258"/>
+        <v>7</v>
+      </c>
+      <c r="F1737">
+        <f t="shared" si="259"/>
+        <v>2023</v>
+      </c>
+      <c r="G1737">
+        <f t="shared" si="260"/>
+        <v>3</v>
+      </c>
+      <c r="H1737" t="str">
+        <f t="shared" si="261"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="I1737" t="str">
+        <f t="shared" si="262"/>
+        <v>Jul</v>
+      </c>
+      <c r="J1737" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1738" s="1">
+        <v>45143</v>
+      </c>
+      <c r="B1738" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1738" t="s">
+        <v>984</v>
+      </c>
+      <c r="D1738">
+        <v>7.99</v>
+      </c>
+      <c r="E1738">
+        <f t="shared" si="258"/>
+        <v>8</v>
+      </c>
+      <c r="F1738">
+        <f t="shared" si="259"/>
+        <v>2023</v>
+      </c>
+      <c r="G1738">
+        <f t="shared" si="260"/>
+        <v>6</v>
+      </c>
+      <c r="H1738" t="str">
+        <f t="shared" si="261"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1738" t="str">
+        <f t="shared" si="262"/>
+        <v>Aug</v>
+      </c>
+      <c r="J1738" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1739" s="1">
+        <v>45174</v>
+      </c>
+      <c r="B1739" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1739" t="s">
+        <v>984</v>
+      </c>
+      <c r="D1739">
+        <v>7.99</v>
+      </c>
+      <c r="E1739">
+        <f t="shared" si="258"/>
+        <v>9</v>
+      </c>
+      <c r="F1739">
+        <f t="shared" si="259"/>
+        <v>2023</v>
+      </c>
+      <c r="G1739">
+        <f t="shared" si="260"/>
+        <v>2</v>
+      </c>
+      <c r="H1739" t="str">
+        <f t="shared" si="261"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1739" t="str">
+        <f t="shared" si="262"/>
+        <v>Sep</v>
+      </c>
+      <c r="J1739" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1740" s="1">
+        <v>45204</v>
+      </c>
+      <c r="B1740" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1740" t="s">
+        <v>984</v>
+      </c>
+      <c r="D1740">
+        <v>7.99</v>
+      </c>
+      <c r="E1740">
+        <f t="shared" si="258"/>
+        <v>10</v>
+      </c>
+      <c r="F1740">
+        <f t="shared" si="259"/>
+        <v>2023</v>
+      </c>
+      <c r="G1740">
+        <f t="shared" si="260"/>
+        <v>4</v>
+      </c>
+      <c r="H1740" t="str">
+        <f t="shared" si="261"/>
+        <v>Thursday</v>
+      </c>
+      <c r="I1740" t="str">
+        <f t="shared" si="262"/>
+        <v>Oct</v>
+      </c>
+      <c r="J1740" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1741" s="1">
+        <v>45235</v>
+      </c>
+      <c r="B1741" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1741" t="s">
+        <v>984</v>
+      </c>
+      <c r="D1741">
+        <v>7.99</v>
+      </c>
+      <c r="E1741">
+        <f t="shared" si="258"/>
+        <v>11</v>
+      </c>
+      <c r="F1741">
+        <f t="shared" si="259"/>
+        <v>2023</v>
+      </c>
+      <c r="G1741">
+        <f t="shared" si="260"/>
+        <v>7</v>
+      </c>
+      <c r="H1741" t="str">
+        <f t="shared" si="261"/>
+        <v>Sunday</v>
+      </c>
+      <c r="I1741" t="str">
+        <f t="shared" si="262"/>
+        <v>Nov</v>
+      </c>
+      <c r="J1741" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1742" s="1">
+        <v>45265</v>
+      </c>
+      <c r="B1742" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1742" t="s">
+        <v>984</v>
+      </c>
+      <c r="D1742">
+        <v>7.99</v>
+      </c>
+      <c r="E1742">
+        <f t="shared" si="258"/>
+        <v>12</v>
+      </c>
+      <c r="F1742">
+        <f t="shared" si="259"/>
+        <v>2023</v>
+      </c>
+      <c r="G1742">
+        <f t="shared" si="260"/>
+        <v>2</v>
+      </c>
+      <c r="H1742" t="str">
+        <f t="shared" si="261"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1742" t="str">
+        <f t="shared" si="262"/>
+        <v>Dec</v>
+      </c>
+      <c r="J1742" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1743" s="1">
+        <v>45296</v>
+      </c>
+      <c r="B1743" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1743" t="s">
+        <v>984</v>
+      </c>
+      <c r="D1743">
+        <v>7.99</v>
+      </c>
+      <c r="E1743">
+        <f t="shared" si="258"/>
+        <v>1</v>
+      </c>
+      <c r="F1743">
+        <f t="shared" si="259"/>
+        <v>2024</v>
+      </c>
+      <c r="G1743">
+        <f t="shared" si="260"/>
+        <v>5</v>
+      </c>
+      <c r="H1743" t="str">
+        <f t="shared" si="261"/>
+        <v>Friday</v>
+      </c>
+      <c r="I1743" t="str">
+        <f t="shared" si="262"/>
+        <v>Jan</v>
+      </c>
+      <c r="J1743" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="1744" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1744" s="1">
+        <v>45327</v>
+      </c>
+      <c r="B1744" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1744" t="s">
+        <v>984</v>
+      </c>
+      <c r="D1744">
+        <v>7.99</v>
+      </c>
+      <c r="E1744">
+        <f t="shared" si="258"/>
+        <v>2</v>
+      </c>
+      <c r="F1744">
+        <f t="shared" si="259"/>
+        <v>2024</v>
+      </c>
+      <c r="G1744">
+        <f t="shared" si="260"/>
+        <v>1</v>
+      </c>
+      <c r="H1744" t="str">
+        <f t="shared" si="261"/>
+        <v>Monday</v>
+      </c>
+      <c r="I1744" t="str">
+        <f t="shared" si="262"/>
+        <v>Feb</v>
+      </c>
+      <c r="J1744" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="1745" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1745" s="1">
+        <v>45356</v>
+      </c>
+      <c r="B1745" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1745" t="s">
+        <v>984</v>
+      </c>
+      <c r="D1745">
+        <v>7.99</v>
+      </c>
+      <c r="E1745">
+        <f t="shared" si="258"/>
+        <v>3</v>
+      </c>
+      <c r="F1745">
+        <f t="shared" si="259"/>
+        <v>2024</v>
+      </c>
+      <c r="G1745">
+        <f t="shared" si="260"/>
+        <v>2</v>
+      </c>
+      <c r="H1745" t="str">
+        <f t="shared" si="261"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1745" t="str">
+        <f t="shared" si="262"/>
+        <v>Mar</v>
+      </c>
+      <c r="J1745" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="1746" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1746" s="1">
+        <v>45387</v>
+      </c>
+      <c r="B1746" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1746" t="s">
+        <v>984</v>
+      </c>
+      <c r="D1746">
+        <v>7.99</v>
+      </c>
+      <c r="E1746">
+        <f t="shared" si="258"/>
+        <v>4</v>
+      </c>
+      <c r="F1746">
+        <f t="shared" si="259"/>
+        <v>2024</v>
+      </c>
+      <c r="G1746">
+        <f t="shared" si="260"/>
+        <v>5</v>
+      </c>
+      <c r="H1746" t="str">
+        <f t="shared" si="261"/>
+        <v>Friday</v>
+      </c>
+      <c r="I1746" t="str">
+        <f t="shared" si="262"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1746" t="s">
+        <v>985</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add: add expenses for the end of April
</commit_message>
<xml_diff>
--- a/data/expense_tracker.xlsx
+++ b/data/expense_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\solutions\learning_python\expense_tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A394EEC-3430-42DF-BD06-B89BCDED0A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EDA535-3CE7-4F94-9A83-49CAEC66042B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" xr2:uid="{7A62D1F9-0105-4F41-8BB8-21CA3D721AF6}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="9" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">total!$A$1:$L$1724</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">total!$A$1:$L$1803</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6429" uniqueCount="986">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6732" uniqueCount="1030">
   <si>
     <t>expense_type</t>
   </si>
@@ -2998,6 +2998,138 @@
   </si>
   <si>
     <t>netflix</t>
+  </si>
+  <si>
+    <t>sparheuminatur 500g</t>
+  </si>
+  <si>
+    <t>sbudget p-geschnetz</t>
+  </si>
+  <si>
+    <t>prem. bio zwiebel</t>
+  </si>
+  <si>
+    <t>veggie pitabrot 400g</t>
+  </si>
+  <si>
+    <t>sbudget kokosmilch</t>
+  </si>
+  <si>
+    <t>sbudgetjo1%500g</t>
+  </si>
+  <si>
+    <t>sbudget eier bh m</t>
+  </si>
+  <si>
+    <t>sbudget langk.reis</t>
+  </si>
+  <si>
+    <t>shan shi yellowcurry</t>
+  </si>
+  <si>
+    <t>sbu paprika mix</t>
+  </si>
+  <si>
+    <t>spar bio zwiebel</t>
+  </si>
+  <si>
+    <t>bermuda chino</t>
+  </si>
+  <si>
+    <t>kleider bauer</t>
+  </si>
+  <si>
+    <t>apfel tasse evelina</t>
+  </si>
+  <si>
+    <t>sriracha saucen</t>
+  </si>
+  <si>
+    <t>bananen chiquita 0.550kgx2,29 eur/kg</t>
+  </si>
+  <si>
+    <t>sbudget gurken 670g</t>
+  </si>
+  <si>
+    <t>suntat gefullte</t>
+  </si>
+  <si>
+    <t>tramezzino</t>
+  </si>
+  <si>
+    <t>la gestione srl</t>
+  </si>
+  <si>
+    <t>marghera</t>
+  </si>
+  <si>
+    <t>t pam nespresso deca</t>
+  </si>
+  <si>
+    <t>ark det liq aloe</t>
+  </si>
+  <si>
+    <t>ark det liq clas</t>
+  </si>
+  <si>
+    <t>ark det liq igie</t>
+  </si>
+  <si>
+    <t>new parodontax com</t>
+  </si>
+  <si>
+    <t>parodontax comp pr</t>
+  </si>
+  <si>
+    <t>v meridol alito fre</t>
+  </si>
+  <si>
+    <t>dent. Parodontax</t>
+  </si>
+  <si>
+    <t>transito</t>
+  </si>
+  <si>
+    <t>ali</t>
+  </si>
+  <si>
+    <t>acqua easy nat.s.benedetto lt1</t>
+  </si>
+  <si>
+    <t>parcheggio</t>
+  </si>
+  <si>
+    <t>venezia mestre</t>
+  </si>
+  <si>
+    <t>avm holding</t>
+  </si>
+  <si>
+    <t>odstore</t>
+  </si>
+  <si>
+    <t>valigetta amaretti e vino</t>
+  </si>
+  <si>
+    <t>torroncini assortiti 250g</t>
+  </si>
+  <si>
+    <t>don peppe</t>
+  </si>
+  <si>
+    <t>pizza rustichella</t>
+  </si>
+  <si>
+    <t>naturale cl. 50</t>
+  </si>
+  <si>
+    <t>caffe espresso</t>
+  </si>
+  <si>
+    <t>sf mozza. Light</t>
+  </si>
+  <si>
+    <t>best moments 85%</t>
   </si>
 </sst>
 </file>
@@ -3350,11 +3482,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397426C9-9494-4E73-BF9B-2DE40DB1433B}">
-  <dimension ref="A1:L1746"/>
+  <dimension ref="A1:L1824"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1728" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1737" sqref="J1737:J1746"/>
+      <pane ySplit="1" topLeftCell="A1801" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1810" sqref="I1810"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -66853,23 +66985,23 @@
         <v>7.99</v>
       </c>
       <c r="E1736">
-        <f t="shared" ref="E1736:E1746" si="258">MONTH(A1736)</f>
+        <f t="shared" ref="E1736:E1747" si="258">MONTH(A1736)</f>
         <v>6</v>
       </c>
       <c r="F1736">
-        <f t="shared" ref="F1736:F1746" si="259">YEAR(A1736)</f>
+        <f t="shared" ref="F1736:F1747" si="259">YEAR(A1736)</f>
         <v>2023</v>
       </c>
       <c r="G1736">
-        <f t="shared" ref="G1736:G1746" si="260">WEEKDAY(A1736, 2)</f>
+        <f t="shared" ref="G1736:G1747" si="260">WEEKDAY(A1736, 2)</f>
         <v>1</v>
       </c>
       <c r="H1736" t="str">
-        <f t="shared" ref="H1736:H1746" si="261">CHOOSE(WEEKDAY(A1736, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <f t="shared" ref="H1736:H1747" si="261">CHOOSE(WEEKDAY(A1736, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
         <v>Monday</v>
       </c>
       <c r="I1736" t="str">
-        <f t="shared" ref="I1736:I1746" si="262">TEXT(A1736, "MMM")</f>
+        <f t="shared" ref="I1736:I1747" si="262">TEXT(A1736, "MMM")</f>
         <v>Jun</v>
       </c>
       <c r="J1736" t="s">
@@ -67172,7 +67304,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="1745" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1745" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1745" s="1">
         <v>45356</v>
       </c>
@@ -67209,7 +67341,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="1746" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1746" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1746" s="1">
         <v>45387</v>
       </c>
@@ -67246,7 +67378,3122 @@
         <v>985</v>
       </c>
     </row>
+    <row r="1747" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1747" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B1747" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1747" t="s">
+        <v>986</v>
+      </c>
+      <c r="D1747">
+        <v>0.89</v>
+      </c>
+      <c r="E1747">
+        <f t="shared" si="258"/>
+        <v>4</v>
+      </c>
+      <c r="F1747">
+        <f t="shared" si="259"/>
+        <v>2024</v>
+      </c>
+      <c r="G1747">
+        <f t="shared" si="260"/>
+        <v>6</v>
+      </c>
+      <c r="H1747" t="str">
+        <f t="shared" si="261"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1747" t="str">
+        <f t="shared" si="262"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1747" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="1748" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1748" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B1748" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1748" t="s">
+        <v>986</v>
+      </c>
+      <c r="D1748">
+        <v>0.89</v>
+      </c>
+      <c r="E1748">
+        <f t="shared" ref="E1748" si="263">MONTH(A1748)</f>
+        <v>4</v>
+      </c>
+      <c r="F1748">
+        <f t="shared" ref="F1748" si="264">YEAR(A1748)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1748">
+        <f t="shared" ref="G1748" si="265">WEEKDAY(A1748, 2)</f>
+        <v>6</v>
+      </c>
+      <c r="H1748" t="str">
+        <f t="shared" ref="H1748" si="266">CHOOSE(WEEKDAY(A1748, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Saturday</v>
+      </c>
+      <c r="I1748" t="str">
+        <f t="shared" ref="I1748" si="267">TEXT(A1748, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1748" t="s">
+        <v>973</v>
+      </c>
+      <c r="K1748" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1749" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1749" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B1749" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1749" t="s">
+        <v>987</v>
+      </c>
+      <c r="D1749">
+        <v>3.99</v>
+      </c>
+      <c r="E1749">
+        <f t="shared" ref="E1749:E1755" si="268">MONTH(A1749)</f>
+        <v>4</v>
+      </c>
+      <c r="F1749">
+        <f t="shared" ref="F1749:F1755" si="269">YEAR(A1749)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1749">
+        <f t="shared" ref="G1749:G1755" si="270">WEEKDAY(A1749, 2)</f>
+        <v>6</v>
+      </c>
+      <c r="H1749" t="str">
+        <f t="shared" ref="H1749:H1755" si="271">CHOOSE(WEEKDAY(A1749, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Saturday</v>
+      </c>
+      <c r="I1749" t="str">
+        <f t="shared" ref="I1749:I1755" si="272">TEXT(A1749, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1749" t="s">
+        <v>973</v>
+      </c>
+      <c r="K1749" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1750" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1750" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B1750" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1750" t="s">
+        <v>352</v>
+      </c>
+      <c r="D1750">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="E1750">
+        <f t="shared" si="268"/>
+        <v>4</v>
+      </c>
+      <c r="F1750">
+        <f t="shared" si="269"/>
+        <v>2024</v>
+      </c>
+      <c r="G1750">
+        <f t="shared" si="270"/>
+        <v>6</v>
+      </c>
+      <c r="H1750" t="str">
+        <f t="shared" si="271"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1750" t="str">
+        <f t="shared" si="272"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1750" t="s">
+        <v>973</v>
+      </c>
+      <c r="K1750" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1751" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1751" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B1751" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1751" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1751">
+        <v>1.99</v>
+      </c>
+      <c r="E1751">
+        <f t="shared" si="268"/>
+        <v>4</v>
+      </c>
+      <c r="F1751">
+        <f t="shared" si="269"/>
+        <v>2024</v>
+      </c>
+      <c r="G1751">
+        <f t="shared" si="270"/>
+        <v>6</v>
+      </c>
+      <c r="H1751" t="str">
+        <f t="shared" si="271"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1751" t="str">
+        <f t="shared" si="272"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1751" t="s">
+        <v>973</v>
+      </c>
+      <c r="K1751" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1752" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1752" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B1752" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1752" t="s">
+        <v>988</v>
+      </c>
+      <c r="D1752">
+        <v>3.99</v>
+      </c>
+      <c r="E1752">
+        <f t="shared" si="268"/>
+        <v>4</v>
+      </c>
+      <c r="F1752">
+        <f t="shared" si="269"/>
+        <v>2024</v>
+      </c>
+      <c r="G1752">
+        <f t="shared" si="270"/>
+        <v>6</v>
+      </c>
+      <c r="H1752" t="str">
+        <f t="shared" si="271"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1752" t="str">
+        <f t="shared" si="272"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1752" t="s">
+        <v>973</v>
+      </c>
+      <c r="K1752" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1753" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1753" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B1753" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1753" t="s">
+        <v>989</v>
+      </c>
+      <c r="D1753">
+        <f>1.89-0.475</f>
+        <v>1.415</v>
+      </c>
+      <c r="E1753">
+        <f t="shared" si="268"/>
+        <v>4</v>
+      </c>
+      <c r="F1753">
+        <f t="shared" si="269"/>
+        <v>2024</v>
+      </c>
+      <c r="G1753">
+        <f t="shared" si="270"/>
+        <v>6</v>
+      </c>
+      <c r="H1753" t="str">
+        <f t="shared" si="271"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1753" t="str">
+        <f t="shared" si="272"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1753" t="s">
+        <v>973</v>
+      </c>
+      <c r="K1753" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1754" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1754" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B1754" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1754" t="s">
+        <v>989</v>
+      </c>
+      <c r="D1754">
+        <f>1.89-0.475</f>
+        <v>1.415</v>
+      </c>
+      <c r="E1754">
+        <f t="shared" si="268"/>
+        <v>4</v>
+      </c>
+      <c r="F1754">
+        <f t="shared" si="269"/>
+        <v>2024</v>
+      </c>
+      <c r="G1754">
+        <f t="shared" si="270"/>
+        <v>6</v>
+      </c>
+      <c r="H1754" t="str">
+        <f t="shared" si="271"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1754" t="str">
+        <f t="shared" si="272"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1754" t="s">
+        <v>973</v>
+      </c>
+      <c r="K1754" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1755" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1755" s="1">
+        <v>45408</v>
+      </c>
+      <c r="B1755" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1755" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1755">
+        <v>4.16</v>
+      </c>
+      <c r="E1755">
+        <f t="shared" si="268"/>
+        <v>4</v>
+      </c>
+      <c r="F1755">
+        <f t="shared" si="269"/>
+        <v>2024</v>
+      </c>
+      <c r="G1755">
+        <f t="shared" si="270"/>
+        <v>5</v>
+      </c>
+      <c r="H1755" t="str">
+        <f t="shared" si="271"/>
+        <v>Friday</v>
+      </c>
+      <c r="I1755" t="str">
+        <f t="shared" si="272"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1755" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1756" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1756" s="1">
+        <v>45408</v>
+      </c>
+      <c r="B1756" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1756" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1756">
+        <v>0.79</v>
+      </c>
+      <c r="E1756">
+        <f t="shared" ref="E1756" si="273">MONTH(A1756)</f>
+        <v>4</v>
+      </c>
+      <c r="F1756">
+        <f t="shared" ref="F1756" si="274">YEAR(A1756)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1756">
+        <f t="shared" ref="G1756" si="275">WEEKDAY(A1756, 2)</f>
+        <v>5</v>
+      </c>
+      <c r="H1756" t="str">
+        <f t="shared" ref="H1756" si="276">CHOOSE(WEEKDAY(A1756, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Friday</v>
+      </c>
+      <c r="I1756" t="str">
+        <f t="shared" ref="I1756" si="277">TEXT(A1756, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1756" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1757" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1757" s="1">
+        <v>45405</v>
+      </c>
+      <c r="B1757" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1757" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1757">
+        <v>2.9</v>
+      </c>
+      <c r="E1757">
+        <f t="shared" ref="E1757:E1760" si="278">MONTH(A1757)</f>
+        <v>4</v>
+      </c>
+      <c r="F1757">
+        <f t="shared" ref="F1757:F1760" si="279">YEAR(A1757)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1757">
+        <f t="shared" ref="G1757:G1760" si="280">WEEKDAY(A1757, 2)</f>
+        <v>2</v>
+      </c>
+      <c r="H1757" t="str">
+        <f t="shared" ref="H1757:H1760" si="281">CHOOSE(WEEKDAY(A1757, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1757" t="str">
+        <f t="shared" ref="I1757:I1760" si="282">TEXT(A1757, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1757" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1758" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1758" s="1">
+        <v>45406</v>
+      </c>
+      <c r="B1758" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1758" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1758">
+        <v>2.9</v>
+      </c>
+      <c r="E1758">
+        <f t="shared" si="278"/>
+        <v>4</v>
+      </c>
+      <c r="F1758">
+        <f t="shared" si="279"/>
+        <v>2024</v>
+      </c>
+      <c r="G1758">
+        <f t="shared" si="280"/>
+        <v>3</v>
+      </c>
+      <c r="H1758" t="str">
+        <f t="shared" si="281"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="I1758" t="str">
+        <f t="shared" si="282"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1758" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1759" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1759" s="1">
+        <v>45404</v>
+      </c>
+      <c r="B1759" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1759" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1759">
+        <v>2.9</v>
+      </c>
+      <c r="E1759">
+        <f t="shared" si="278"/>
+        <v>4</v>
+      </c>
+      <c r="F1759">
+        <f t="shared" si="279"/>
+        <v>2024</v>
+      </c>
+      <c r="G1759">
+        <f t="shared" si="280"/>
+        <v>1</v>
+      </c>
+      <c r="H1759" t="str">
+        <f t="shared" si="281"/>
+        <v>Monday</v>
+      </c>
+      <c r="I1759" t="str">
+        <f t="shared" si="282"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1759" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1760" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1760" s="1">
+        <v>45412</v>
+      </c>
+      <c r="B1760" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1760" t="s">
+        <v>990</v>
+      </c>
+      <c r="D1760">
+        <v>0.99</v>
+      </c>
+      <c r="E1760">
+        <f t="shared" si="278"/>
+        <v>4</v>
+      </c>
+      <c r="F1760">
+        <f t="shared" si="279"/>
+        <v>2024</v>
+      </c>
+      <c r="G1760">
+        <f t="shared" si="280"/>
+        <v>2</v>
+      </c>
+      <c r="H1760" t="str">
+        <f t="shared" si="281"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1760" t="str">
+        <f t="shared" si="282"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1760" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1760" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1761" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1761" s="1">
+        <v>45412</v>
+      </c>
+      <c r="B1761" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1761" t="s">
+        <v>969</v>
+      </c>
+      <c r="D1761">
+        <f>2.99-0.75</f>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="E1761">
+        <f t="shared" ref="E1761:E1767" si="283">MONTH(A1761)</f>
+        <v>4</v>
+      </c>
+      <c r="F1761">
+        <f t="shared" ref="F1761:F1767" si="284">YEAR(A1761)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1761">
+        <f t="shared" ref="G1761:G1767" si="285">WEEKDAY(A1761, 2)</f>
+        <v>2</v>
+      </c>
+      <c r="H1761" t="str">
+        <f t="shared" ref="H1761:H1767" si="286">CHOOSE(WEEKDAY(A1761, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1761" t="str">
+        <f t="shared" ref="I1761:I1767" si="287">TEXT(A1761, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1761" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1761" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1762" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1762" s="1">
+        <v>45412</v>
+      </c>
+      <c r="B1762" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1762" t="s">
+        <v>991</v>
+      </c>
+      <c r="D1762">
+        <v>0.79</v>
+      </c>
+      <c r="E1762">
+        <f t="shared" si="283"/>
+        <v>4</v>
+      </c>
+      <c r="F1762">
+        <f t="shared" si="284"/>
+        <v>2024</v>
+      </c>
+      <c r="G1762">
+        <f t="shared" si="285"/>
+        <v>2</v>
+      </c>
+      <c r="H1762" t="str">
+        <f t="shared" si="286"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1762" t="str">
+        <f t="shared" si="287"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1762" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1762" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1763" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1763" s="1">
+        <v>45412</v>
+      </c>
+      <c r="B1763" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1763" t="s">
+        <v>992</v>
+      </c>
+      <c r="D1763">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="E1763">
+        <f t="shared" si="283"/>
+        <v>4</v>
+      </c>
+      <c r="F1763">
+        <f t="shared" si="284"/>
+        <v>2024</v>
+      </c>
+      <c r="G1763">
+        <f t="shared" si="285"/>
+        <v>2</v>
+      </c>
+      <c r="H1763" t="str">
+        <f t="shared" si="286"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1763" t="str">
+        <f t="shared" si="287"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1763" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1763" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1764" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1764" s="1">
+        <v>45412</v>
+      </c>
+      <c r="B1764" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1764" t="s">
+        <v>993</v>
+      </c>
+      <c r="D1764">
+        <v>1.19</v>
+      </c>
+      <c r="E1764">
+        <f t="shared" si="283"/>
+        <v>4</v>
+      </c>
+      <c r="F1764">
+        <f t="shared" si="284"/>
+        <v>2024</v>
+      </c>
+      <c r="G1764">
+        <f t="shared" si="285"/>
+        <v>2</v>
+      </c>
+      <c r="H1764" t="str">
+        <f t="shared" si="286"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1764" t="str">
+        <f t="shared" si="287"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1764" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1764" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1765" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1765" s="1">
+        <v>45412</v>
+      </c>
+      <c r="B1765" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1765" t="s">
+        <v>994</v>
+      </c>
+      <c r="D1765">
+        <f>2.99-0.75</f>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="E1765">
+        <f t="shared" si="283"/>
+        <v>4</v>
+      </c>
+      <c r="F1765">
+        <f t="shared" si="284"/>
+        <v>2024</v>
+      </c>
+      <c r="G1765">
+        <f t="shared" si="285"/>
+        <v>2</v>
+      </c>
+      <c r="H1765" t="str">
+        <f t="shared" si="286"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1765" t="str">
+        <f t="shared" si="287"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1765" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1765" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1766" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1766" s="1">
+        <v>45412</v>
+      </c>
+      <c r="B1766" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1766" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1766">
+        <f>5.99-1.5</f>
+        <v>4.49</v>
+      </c>
+      <c r="E1766">
+        <f t="shared" si="283"/>
+        <v>4</v>
+      </c>
+      <c r="F1766">
+        <f t="shared" si="284"/>
+        <v>2024</v>
+      </c>
+      <c r="G1766">
+        <f t="shared" si="285"/>
+        <v>2</v>
+      </c>
+      <c r="H1766" t="str">
+        <f t="shared" si="286"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1766" t="str">
+        <f t="shared" si="287"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1766" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1766" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1767" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1767" s="1">
+        <v>45412</v>
+      </c>
+      <c r="B1767" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1767" t="s">
+        <v>995</v>
+      </c>
+      <c r="D1767">
+        <v>1.99</v>
+      </c>
+      <c r="E1767">
+        <f t="shared" si="283"/>
+        <v>4</v>
+      </c>
+      <c r="F1767">
+        <f t="shared" si="284"/>
+        <v>2024</v>
+      </c>
+      <c r="G1767">
+        <f t="shared" si="285"/>
+        <v>2</v>
+      </c>
+      <c r="H1767" t="str">
+        <f t="shared" si="286"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1767" t="str">
+        <f t="shared" si="287"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1767" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1767" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1768" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1768" s="1">
+        <v>45412</v>
+      </c>
+      <c r="B1768" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1768" t="s">
+        <v>248</v>
+      </c>
+      <c r="D1768">
+        <v>1.44</v>
+      </c>
+      <c r="E1768">
+        <f t="shared" ref="E1768:E1772" si="288">MONTH(A1768)</f>
+        <v>4</v>
+      </c>
+      <c r="F1768">
+        <f t="shared" ref="F1768:F1772" si="289">YEAR(A1768)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1768">
+        <f t="shared" ref="G1768:G1772" si="290">WEEKDAY(A1768, 2)</f>
+        <v>2</v>
+      </c>
+      <c r="H1768" t="str">
+        <f t="shared" ref="H1768:H1772" si="291">CHOOSE(WEEKDAY(A1768, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1768" t="str">
+        <f t="shared" ref="I1768:I1772" si="292">TEXT(A1768, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1768" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1768" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1769" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1769" s="1">
+        <v>45412</v>
+      </c>
+      <c r="B1769" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1769" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1769">
+        <v>1.99</v>
+      </c>
+      <c r="E1769">
+        <f t="shared" si="288"/>
+        <v>4</v>
+      </c>
+      <c r="F1769">
+        <f t="shared" si="289"/>
+        <v>2024</v>
+      </c>
+      <c r="G1769">
+        <f t="shared" si="290"/>
+        <v>2</v>
+      </c>
+      <c r="H1769" t="str">
+        <f t="shared" si="291"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1769" t="str">
+        <f t="shared" si="292"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1769" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1769" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1770" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1770" s="1">
+        <v>45412</v>
+      </c>
+      <c r="B1770" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1770" t="s">
+        <v>996</v>
+      </c>
+      <c r="D1770">
+        <f>2.19-0.55</f>
+        <v>1.64</v>
+      </c>
+      <c r="E1770">
+        <f t="shared" si="288"/>
+        <v>4</v>
+      </c>
+      <c r="F1770">
+        <f t="shared" si="289"/>
+        <v>2024</v>
+      </c>
+      <c r="G1770">
+        <f t="shared" si="290"/>
+        <v>2</v>
+      </c>
+      <c r="H1770" t="str">
+        <f t="shared" si="291"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1770" t="str">
+        <f t="shared" si="292"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1770" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1770" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1771" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1771" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B1771" t="s">
+        <v>303</v>
+      </c>
+      <c r="C1771" t="s">
+        <v>997</v>
+      </c>
+      <c r="D1771">
+        <v>24.6</v>
+      </c>
+      <c r="E1771">
+        <f t="shared" si="288"/>
+        <v>4</v>
+      </c>
+      <c r="F1771">
+        <f t="shared" si="289"/>
+        <v>2024</v>
+      </c>
+      <c r="G1771">
+        <f t="shared" si="290"/>
+        <v>6</v>
+      </c>
+      <c r="H1771" t="str">
+        <f t="shared" si="291"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1771" t="str">
+        <f t="shared" si="292"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1771" t="s">
+        <v>998</v>
+      </c>
+      <c r="K1771" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="1772" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1772" s="1">
+        <v>45404</v>
+      </c>
+      <c r="B1772" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1772" t="s">
+        <v>845</v>
+      </c>
+      <c r="D1772">
+        <v>0.59</v>
+      </c>
+      <c r="E1772">
+        <f t="shared" si="288"/>
+        <v>4</v>
+      </c>
+      <c r="F1772">
+        <f t="shared" si="289"/>
+        <v>2024</v>
+      </c>
+      <c r="G1772">
+        <f t="shared" si="290"/>
+        <v>1</v>
+      </c>
+      <c r="H1772" t="str">
+        <f t="shared" si="291"/>
+        <v>Monday</v>
+      </c>
+      <c r="I1772" t="str">
+        <f t="shared" si="292"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1772" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1772" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="1773" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1773" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B1773" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1773" t="s">
+        <v>530</v>
+      </c>
+      <c r="D1773">
+        <v>1.29</v>
+      </c>
+      <c r="E1773">
+        <f t="shared" ref="E1773:E1780" si="293">MONTH(A1773)</f>
+        <v>4</v>
+      </c>
+      <c r="F1773">
+        <f t="shared" ref="F1773:F1780" si="294">YEAR(A1773)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1773">
+        <f t="shared" ref="G1773:G1780" si="295">WEEKDAY(A1773, 2)</f>
+        <v>6</v>
+      </c>
+      <c r="H1773" t="str">
+        <f t="shared" ref="H1773:H1780" si="296">CHOOSE(WEEKDAY(A1773, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Saturday</v>
+      </c>
+      <c r="I1773" t="str">
+        <f t="shared" ref="I1773:I1780" si="297">TEXT(A1773, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1773" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1773" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1774" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1774" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B1774" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1774" t="s">
+        <v>847</v>
+      </c>
+      <c r="D1774">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="E1774">
+        <f t="shared" si="293"/>
+        <v>4</v>
+      </c>
+      <c r="F1774">
+        <f t="shared" si="294"/>
+        <v>2024</v>
+      </c>
+      <c r="G1774">
+        <f t="shared" si="295"/>
+        <v>6</v>
+      </c>
+      <c r="H1774" t="str">
+        <f t="shared" si="296"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1774" t="str">
+        <f t="shared" si="297"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1774" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1774" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1775" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1775" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B1775" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1775" t="s">
+        <v>999</v>
+      </c>
+      <c r="D1775">
+        <v>2.06</v>
+      </c>
+      <c r="E1775">
+        <f t="shared" si="293"/>
+        <v>4</v>
+      </c>
+      <c r="F1775">
+        <f t="shared" si="294"/>
+        <v>2024</v>
+      </c>
+      <c r="G1775">
+        <f t="shared" si="295"/>
+        <v>6</v>
+      </c>
+      <c r="H1775" t="str">
+        <f t="shared" si="296"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1775" t="str">
+        <f t="shared" si="297"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1775" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1775" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1776" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1776" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B1776" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1776" t="s">
+        <v>911</v>
+      </c>
+      <c r="D1776">
+        <f>2.89-0.7</f>
+        <v>2.1900000000000004</v>
+      </c>
+      <c r="E1776">
+        <f t="shared" si="293"/>
+        <v>4</v>
+      </c>
+      <c r="F1776">
+        <f t="shared" si="294"/>
+        <v>2024</v>
+      </c>
+      <c r="G1776">
+        <f t="shared" si="295"/>
+        <v>6</v>
+      </c>
+      <c r="H1776" t="str">
+        <f t="shared" si="296"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1776" t="str">
+        <f t="shared" si="297"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1776" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1776" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1777" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1777" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B1777" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1777" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D1777">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="E1777">
+        <f t="shared" si="293"/>
+        <v>4</v>
+      </c>
+      <c r="F1777">
+        <f t="shared" si="294"/>
+        <v>2024</v>
+      </c>
+      <c r="G1777">
+        <f t="shared" si="295"/>
+        <v>6</v>
+      </c>
+      <c r="H1777" t="str">
+        <f t="shared" si="296"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1777" t="str">
+        <f t="shared" si="297"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1777" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1777" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1778" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1778" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B1778" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1778" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D1778">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="E1778">
+        <f t="shared" si="293"/>
+        <v>4</v>
+      </c>
+      <c r="F1778">
+        <f t="shared" si="294"/>
+        <v>2024</v>
+      </c>
+      <c r="G1778">
+        <f t="shared" si="295"/>
+        <v>6</v>
+      </c>
+      <c r="H1778" t="str">
+        <f t="shared" si="296"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1778" t="str">
+        <f t="shared" si="297"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1778" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1778" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1779" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1779" s="1">
+        <v>45402</v>
+      </c>
+      <c r="B1779" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1779" t="s">
+        <v>737</v>
+      </c>
+      <c r="D1779">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="E1779">
+        <f t="shared" si="293"/>
+        <v>4</v>
+      </c>
+      <c r="F1779">
+        <f t="shared" si="294"/>
+        <v>2024</v>
+      </c>
+      <c r="G1779">
+        <f t="shared" si="295"/>
+        <v>6</v>
+      </c>
+      <c r="H1779" t="str">
+        <f t="shared" si="296"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1779" t="str">
+        <f t="shared" si="297"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1779" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1779" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1780" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1780" s="1">
+        <v>45408</v>
+      </c>
+      <c r="B1780" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1780" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D1780">
+        <v>1.26</v>
+      </c>
+      <c r="E1780">
+        <f t="shared" si="293"/>
+        <v>4</v>
+      </c>
+      <c r="F1780">
+        <f t="shared" si="294"/>
+        <v>2024</v>
+      </c>
+      <c r="G1780">
+        <f t="shared" si="295"/>
+        <v>5</v>
+      </c>
+      <c r="H1780" t="str">
+        <f t="shared" si="296"/>
+        <v>Friday</v>
+      </c>
+      <c r="I1780" t="str">
+        <f t="shared" si="297"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1780" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1780" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="1781" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1781" s="1">
+        <v>45408</v>
+      </c>
+      <c r="B1781" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1781" t="s">
+        <v>533</v>
+      </c>
+      <c r="D1781">
+        <v>1.58</v>
+      </c>
+      <c r="E1781">
+        <f t="shared" ref="E1781:E1782" si="298">MONTH(A1781)</f>
+        <v>4</v>
+      </c>
+      <c r="F1781">
+        <f t="shared" ref="F1781:F1782" si="299">YEAR(A1781)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1781">
+        <f t="shared" ref="G1781:G1782" si="300">WEEKDAY(A1781, 2)</f>
+        <v>5</v>
+      </c>
+      <c r="H1781" t="str">
+        <f t="shared" ref="H1781:H1782" si="301">CHOOSE(WEEKDAY(A1781, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Friday</v>
+      </c>
+      <c r="I1781" t="str">
+        <f t="shared" ref="I1781:I1782" si="302">TEXT(A1781, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1781" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1781" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="1782" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1782" s="1">
+        <v>45407</v>
+      </c>
+      <c r="B1782" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1782" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1782">
+        <v>0.99</v>
+      </c>
+      <c r="E1782">
+        <f t="shared" si="298"/>
+        <v>4</v>
+      </c>
+      <c r="F1782">
+        <f t="shared" si="299"/>
+        <v>2024</v>
+      </c>
+      <c r="G1782">
+        <f t="shared" si="300"/>
+        <v>4</v>
+      </c>
+      <c r="H1782" t="str">
+        <f t="shared" si="301"/>
+        <v>Thursday</v>
+      </c>
+      <c r="I1782" t="str">
+        <f t="shared" si="302"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1782" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1782" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="1783" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1783" s="1">
+        <v>45407</v>
+      </c>
+      <c r="B1783" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1783" t="s">
+        <v>509</v>
+      </c>
+      <c r="D1783">
+        <v>1.69</v>
+      </c>
+      <c r="E1783">
+        <f t="shared" ref="E1783:E1784" si="303">MONTH(A1783)</f>
+        <v>4</v>
+      </c>
+      <c r="F1783">
+        <f t="shared" ref="F1783:F1784" si="304">YEAR(A1783)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1783">
+        <f t="shared" ref="G1783:G1784" si="305">WEEKDAY(A1783, 2)</f>
+        <v>4</v>
+      </c>
+      <c r="H1783" t="str">
+        <f t="shared" ref="H1783:H1784" si="306">CHOOSE(WEEKDAY(A1783, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Thursday</v>
+      </c>
+      <c r="I1783" t="str">
+        <f t="shared" ref="I1783:I1784" si="307">TEXT(A1783, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1783" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1783" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="1784" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1784" s="1">
+        <v>45408</v>
+      </c>
+      <c r="B1784" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1784" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1784">
+        <v>0.99</v>
+      </c>
+      <c r="E1784">
+        <f t="shared" si="303"/>
+        <v>4</v>
+      </c>
+      <c r="F1784">
+        <f t="shared" si="304"/>
+        <v>2024</v>
+      </c>
+      <c r="G1784">
+        <f t="shared" si="305"/>
+        <v>5</v>
+      </c>
+      <c r="H1784" t="str">
+        <f t="shared" si="306"/>
+        <v>Friday</v>
+      </c>
+      <c r="I1784" t="str">
+        <f t="shared" si="307"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1784" t="s">
+        <v>973</v>
+      </c>
+      <c r="K1784" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="1785" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1785" s="1">
+        <v>45408</v>
+      </c>
+      <c r="B1785" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1785" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1785">
+        <v>0.99</v>
+      </c>
+      <c r="E1785">
+        <f t="shared" ref="E1785:E1788" si="308">MONTH(A1785)</f>
+        <v>4</v>
+      </c>
+      <c r="F1785">
+        <f t="shared" ref="F1785:F1788" si="309">YEAR(A1785)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1785">
+        <f t="shared" ref="G1785:G1788" si="310">WEEKDAY(A1785, 2)</f>
+        <v>5</v>
+      </c>
+      <c r="H1785" t="str">
+        <f t="shared" ref="H1785:H1788" si="311">CHOOSE(WEEKDAY(A1785, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Friday</v>
+      </c>
+      <c r="I1785" t="str">
+        <f t="shared" ref="I1785:I1788" si="312">TEXT(A1785, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1785" t="s">
+        <v>973</v>
+      </c>
+      <c r="K1785" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="1786" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1786" s="1">
+        <v>45408</v>
+      </c>
+      <c r="B1786" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1786" t="s">
+        <v>296</v>
+      </c>
+      <c r="D1786">
+        <v>0.79</v>
+      </c>
+      <c r="E1786">
+        <f t="shared" si="308"/>
+        <v>4</v>
+      </c>
+      <c r="F1786">
+        <f t="shared" si="309"/>
+        <v>2024</v>
+      </c>
+      <c r="G1786">
+        <f t="shared" si="310"/>
+        <v>5</v>
+      </c>
+      <c r="H1786" t="str">
+        <f t="shared" si="311"/>
+        <v>Friday</v>
+      </c>
+      <c r="I1786" t="str">
+        <f t="shared" si="312"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1786" t="s">
+        <v>973</v>
+      </c>
+      <c r="K1786" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="1787" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1787" s="1">
+        <v>45408</v>
+      </c>
+      <c r="B1787" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1787" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D1787">
+        <v>0.99</v>
+      </c>
+      <c r="E1787">
+        <f t="shared" si="308"/>
+        <v>4</v>
+      </c>
+      <c r="F1787">
+        <f t="shared" si="309"/>
+        <v>2024</v>
+      </c>
+      <c r="G1787">
+        <f t="shared" si="310"/>
+        <v>5</v>
+      </c>
+      <c r="H1787" t="str">
+        <f t="shared" si="311"/>
+        <v>Friday</v>
+      </c>
+      <c r="I1787" t="str">
+        <f t="shared" si="312"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1787" t="s">
+        <v>973</v>
+      </c>
+      <c r="K1787" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="1788" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1788" s="1">
+        <v>45408</v>
+      </c>
+      <c r="B1788" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1788" t="s">
+        <v>359</v>
+      </c>
+      <c r="D1788">
+        <v>0.99</v>
+      </c>
+      <c r="E1788">
+        <f t="shared" si="308"/>
+        <v>4</v>
+      </c>
+      <c r="F1788">
+        <f t="shared" si="309"/>
+        <v>2024</v>
+      </c>
+      <c r="G1788">
+        <f t="shared" si="310"/>
+        <v>5</v>
+      </c>
+      <c r="H1788" t="str">
+        <f t="shared" si="311"/>
+        <v>Friday</v>
+      </c>
+      <c r="I1788" t="str">
+        <f t="shared" si="312"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1788" t="s">
+        <v>973</v>
+      </c>
+      <c r="K1788" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="1789" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1789" s="1">
+        <v>45408</v>
+      </c>
+      <c r="B1789" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1789" t="s">
+        <v>971</v>
+      </c>
+      <c r="D1789">
+        <f>1.69-0.43</f>
+        <v>1.26</v>
+      </c>
+      <c r="E1789">
+        <f t="shared" ref="E1789:E1791" si="313">MONTH(A1789)</f>
+        <v>4</v>
+      </c>
+      <c r="F1789">
+        <f t="shared" ref="F1789:F1791" si="314">YEAR(A1789)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1789">
+        <f t="shared" ref="G1789:G1791" si="315">WEEKDAY(A1789, 2)</f>
+        <v>5</v>
+      </c>
+      <c r="H1789" t="str">
+        <f t="shared" ref="H1789:H1791" si="316">CHOOSE(WEEKDAY(A1789, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Friday</v>
+      </c>
+      <c r="I1789" t="str">
+        <f t="shared" ref="I1789:I1791" si="317">TEXT(A1789, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1789" t="s">
+        <v>269</v>
+      </c>
+      <c r="K1789" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="1790" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1790" s="1">
+        <v>45408</v>
+      </c>
+      <c r="B1790" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1790" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D1790">
+        <v>2.85</v>
+      </c>
+      <c r="E1790">
+        <f t="shared" si="313"/>
+        <v>4</v>
+      </c>
+      <c r="F1790">
+        <f t="shared" si="314"/>
+        <v>2024</v>
+      </c>
+      <c r="G1790">
+        <f t="shared" si="315"/>
+        <v>5</v>
+      </c>
+      <c r="H1790" t="str">
+        <f t="shared" si="316"/>
+        <v>Friday</v>
+      </c>
+      <c r="I1790" t="str">
+        <f t="shared" si="317"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1790" t="s">
+        <v>269</v>
+      </c>
+      <c r="K1790" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="1791" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1791" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1791" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1791" t="s">
+        <v>745</v>
+      </c>
+      <c r="D1791">
+        <v>2.6</v>
+      </c>
+      <c r="E1791">
+        <f t="shared" si="313"/>
+        <v>4</v>
+      </c>
+      <c r="F1791">
+        <f t="shared" si="314"/>
+        <v>2024</v>
+      </c>
+      <c r="G1791">
+        <f t="shared" si="315"/>
+        <v>6</v>
+      </c>
+      <c r="H1791" t="str">
+        <f t="shared" si="316"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1791" t="str">
+        <f t="shared" si="317"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1791" t="s">
+        <v>1005</v>
+      </c>
+      <c r="K1791" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="1792" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1792" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1792" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1792" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D1792">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E1792">
+        <f t="shared" ref="E1792" si="318">MONTH(A1792)</f>
+        <v>4</v>
+      </c>
+      <c r="F1792">
+        <f t="shared" ref="F1792" si="319">YEAR(A1792)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1792">
+        <f t="shared" ref="G1792" si="320">WEEKDAY(A1792, 2)</f>
+        <v>6</v>
+      </c>
+      <c r="H1792" t="str">
+        <f t="shared" ref="H1792" si="321">CHOOSE(WEEKDAY(A1792, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Saturday</v>
+      </c>
+      <c r="I1792" t="str">
+        <f t="shared" ref="I1792" si="322">TEXT(A1792, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1792" t="s">
+        <v>1005</v>
+      </c>
+      <c r="K1792" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="1793" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1793" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1793" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1793" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D1793">
+        <v>2</v>
+      </c>
+      <c r="E1793">
+        <f t="shared" ref="E1793:E1803" si="323">MONTH(A1793)</f>
+        <v>4</v>
+      </c>
+      <c r="F1793">
+        <f t="shared" ref="F1793:F1803" si="324">YEAR(A1793)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1793">
+        <f t="shared" ref="G1793:G1803" si="325">WEEKDAY(A1793, 2)</f>
+        <v>6</v>
+      </c>
+      <c r="H1793" t="str">
+        <f t="shared" ref="H1793:H1803" si="326">CHOOSE(WEEKDAY(A1793, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Saturday</v>
+      </c>
+      <c r="I1793" t="str">
+        <f t="shared" ref="I1793:I1803" si="327">TEXT(A1793, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1793" t="s">
+        <v>403</v>
+      </c>
+      <c r="K1793" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="1794" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1794" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1794" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1794" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D1794">
+        <v>2</v>
+      </c>
+      <c r="E1794">
+        <f t="shared" si="323"/>
+        <v>4</v>
+      </c>
+      <c r="F1794">
+        <f t="shared" si="324"/>
+        <v>2024</v>
+      </c>
+      <c r="G1794">
+        <f t="shared" si="325"/>
+        <v>6</v>
+      </c>
+      <c r="H1794" t="str">
+        <f t="shared" si="326"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1794" t="str">
+        <f t="shared" si="327"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1794" t="s">
+        <v>403</v>
+      </c>
+      <c r="K1794" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="1795" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1795" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1795" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1795" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D1795">
+        <v>2</v>
+      </c>
+      <c r="E1795">
+        <f t="shared" si="323"/>
+        <v>4</v>
+      </c>
+      <c r="F1795">
+        <f t="shared" si="324"/>
+        <v>2024</v>
+      </c>
+      <c r="G1795">
+        <f t="shared" si="325"/>
+        <v>6</v>
+      </c>
+      <c r="H1795" t="str">
+        <f t="shared" si="326"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1795" t="str">
+        <f t="shared" si="327"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1795" t="s">
+        <v>403</v>
+      </c>
+      <c r="K1795" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="1796" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1796" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1796" t="s">
+        <v>895</v>
+      </c>
+      <c r="C1796" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D1796">
+        <f>4.2/2</f>
+        <v>2.1</v>
+      </c>
+      <c r="E1796">
+        <f t="shared" si="323"/>
+        <v>4</v>
+      </c>
+      <c r="F1796">
+        <f t="shared" si="324"/>
+        <v>2024</v>
+      </c>
+      <c r="G1796">
+        <f t="shared" si="325"/>
+        <v>6</v>
+      </c>
+      <c r="H1796" t="str">
+        <f t="shared" si="326"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1796" t="str">
+        <f t="shared" si="327"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1796" t="s">
+        <v>403</v>
+      </c>
+      <c r="K1796" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="1797" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1797" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1797" t="s">
+        <v>895</v>
+      </c>
+      <c r="C1797" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D1797">
+        <f>4.2/2</f>
+        <v>2.1</v>
+      </c>
+      <c r="E1797">
+        <f t="shared" si="323"/>
+        <v>4</v>
+      </c>
+      <c r="F1797">
+        <f t="shared" si="324"/>
+        <v>2024</v>
+      </c>
+      <c r="G1797">
+        <f t="shared" si="325"/>
+        <v>6</v>
+      </c>
+      <c r="H1797" t="str">
+        <f t="shared" si="326"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1797" t="str">
+        <f t="shared" si="327"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1797" t="s">
+        <v>403</v>
+      </c>
+      <c r="K1797" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="1798" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1798" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1798" t="s">
+        <v>895</v>
+      </c>
+      <c r="C1798" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D1798">
+        <f>4.2/2</f>
+        <v>2.1</v>
+      </c>
+      <c r="E1798">
+        <f t="shared" si="323"/>
+        <v>4</v>
+      </c>
+      <c r="F1798">
+        <f t="shared" si="324"/>
+        <v>2024</v>
+      </c>
+      <c r="G1798">
+        <f t="shared" si="325"/>
+        <v>6</v>
+      </c>
+      <c r="H1798" t="str">
+        <f t="shared" si="326"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1798" t="str">
+        <f t="shared" si="327"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1798" t="s">
+        <v>403</v>
+      </c>
+      <c r="K1798" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="1799" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1799" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1799" t="s">
+        <v>934</v>
+      </c>
+      <c r="C1799" t="s">
+        <v>1011</v>
+      </c>
+      <c r="D1799">
+        <v>3.7</v>
+      </c>
+      <c r="E1799">
+        <f t="shared" si="323"/>
+        <v>4</v>
+      </c>
+      <c r="F1799">
+        <f t="shared" si="324"/>
+        <v>2024</v>
+      </c>
+      <c r="G1799">
+        <f t="shared" si="325"/>
+        <v>6</v>
+      </c>
+      <c r="H1799" t="str">
+        <f t="shared" si="326"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1799" t="str">
+        <f t="shared" si="327"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1799" t="s">
+        <v>403</v>
+      </c>
+      <c r="K1799" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="1800" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1800" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1800" t="s">
+        <v>934</v>
+      </c>
+      <c r="C1800" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D1800">
+        <v>3.7</v>
+      </c>
+      <c r="E1800">
+        <f t="shared" si="323"/>
+        <v>4</v>
+      </c>
+      <c r="F1800">
+        <f t="shared" si="324"/>
+        <v>2024</v>
+      </c>
+      <c r="G1800">
+        <f t="shared" si="325"/>
+        <v>6</v>
+      </c>
+      <c r="H1800" t="str">
+        <f t="shared" si="326"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1800" t="str">
+        <f t="shared" si="327"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1800" t="s">
+        <v>403</v>
+      </c>
+      <c r="K1800" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="1801" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1801" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1801" t="s">
+        <v>934</v>
+      </c>
+      <c r="C1801" t="s">
+        <v>1013</v>
+      </c>
+      <c r="D1801">
+        <f>5.2-2.6</f>
+        <v>2.6</v>
+      </c>
+      <c r="E1801">
+        <f t="shared" si="323"/>
+        <v>4</v>
+      </c>
+      <c r="F1801">
+        <f t="shared" si="324"/>
+        <v>2024</v>
+      </c>
+      <c r="G1801">
+        <f t="shared" si="325"/>
+        <v>6</v>
+      </c>
+      <c r="H1801" t="str">
+        <f t="shared" si="326"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1801" t="str">
+        <f t="shared" si="327"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1801" t="s">
+        <v>403</v>
+      </c>
+      <c r="K1801" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="1802" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1802" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1802" t="s">
+        <v>934</v>
+      </c>
+      <c r="C1802" t="s">
+        <v>1013</v>
+      </c>
+      <c r="D1802">
+        <f>5.2-2.6</f>
+        <v>2.6</v>
+      </c>
+      <c r="E1802">
+        <f t="shared" si="323"/>
+        <v>4</v>
+      </c>
+      <c r="F1802">
+        <f t="shared" si="324"/>
+        <v>2024</v>
+      </c>
+      <c r="G1802">
+        <f t="shared" si="325"/>
+        <v>6</v>
+      </c>
+      <c r="H1802" t="str">
+        <f t="shared" si="326"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1802" t="str">
+        <f t="shared" si="327"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1802" t="s">
+        <v>403</v>
+      </c>
+      <c r="K1802" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="1803" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1803" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1803" t="s">
+        <v>934</v>
+      </c>
+      <c r="C1803" t="s">
+        <v>1014</v>
+      </c>
+      <c r="D1803">
+        <v>3.7</v>
+      </c>
+      <c r="E1803">
+        <f t="shared" si="323"/>
+        <v>4</v>
+      </c>
+      <c r="F1803">
+        <f t="shared" si="324"/>
+        <v>2024</v>
+      </c>
+      <c r="G1803">
+        <f t="shared" si="325"/>
+        <v>6</v>
+      </c>
+      <c r="H1803" t="str">
+        <f t="shared" si="326"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1803" t="str">
+        <f t="shared" si="327"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1803" t="s">
+        <v>403</v>
+      </c>
+      <c r="K1803" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="1804" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1804" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1804" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1804" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D1804">
+        <f>7.9/2</f>
+        <v>3.95</v>
+      </c>
+      <c r="E1804">
+        <f t="shared" ref="E1804" si="328">MONTH(A1804)</f>
+        <v>4</v>
+      </c>
+      <c r="F1804">
+        <f t="shared" ref="F1804" si="329">YEAR(A1804)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1804">
+        <f t="shared" ref="G1804" si="330">WEEKDAY(A1804, 2)</f>
+        <v>6</v>
+      </c>
+      <c r="H1804" t="str">
+        <f t="shared" ref="H1804" si="331">CHOOSE(WEEKDAY(A1804, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Saturday</v>
+      </c>
+      <c r="I1804" t="str">
+        <f t="shared" ref="I1804" si="332">TEXT(A1804, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1804" t="s">
+        <v>318</v>
+      </c>
+      <c r="K1804" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="1805" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1805" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1805" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1805" t="s">
+        <v>1017</v>
+      </c>
+      <c r="D1805">
+        <v>0.27</v>
+      </c>
+      <c r="E1805">
+        <f t="shared" ref="E1805:E1808" si="333">MONTH(A1805)</f>
+        <v>4</v>
+      </c>
+      <c r="F1805">
+        <f t="shared" ref="F1805:F1808" si="334">YEAR(A1805)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1805">
+        <f t="shared" ref="G1805:G1808" si="335">WEEKDAY(A1805, 2)</f>
+        <v>6</v>
+      </c>
+      <c r="H1805" t="str">
+        <f t="shared" ref="H1805:H1808" si="336">CHOOSE(WEEKDAY(A1805, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Saturday</v>
+      </c>
+      <c r="I1805" t="str">
+        <f t="shared" ref="I1805:I1808" si="337">TEXT(A1805, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1805" t="s">
+        <v>1016</v>
+      </c>
+      <c r="K1805" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="1806" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1806" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1806" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1806" t="s">
+        <v>1017</v>
+      </c>
+      <c r="D1806">
+        <v>0.27</v>
+      </c>
+      <c r="E1806">
+        <f t="shared" si="333"/>
+        <v>4</v>
+      </c>
+      <c r="F1806">
+        <f t="shared" si="334"/>
+        <v>2024</v>
+      </c>
+      <c r="G1806">
+        <f t="shared" si="335"/>
+        <v>6</v>
+      </c>
+      <c r="H1806" t="str">
+        <f t="shared" si="336"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1806" t="str">
+        <f t="shared" si="337"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1806" t="s">
+        <v>1016</v>
+      </c>
+      <c r="K1806" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="1807" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1807" s="1">
+        <v>45411</v>
+      </c>
+      <c r="B1807" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1807" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1807">
+        <v>2.9</v>
+      </c>
+      <c r="E1807">
+        <f t="shared" si="333"/>
+        <v>4</v>
+      </c>
+      <c r="F1807">
+        <f t="shared" si="334"/>
+        <v>2024</v>
+      </c>
+      <c r="G1807">
+        <f t="shared" si="335"/>
+        <v>1</v>
+      </c>
+      <c r="H1807" t="str">
+        <f t="shared" si="336"/>
+        <v>Monday</v>
+      </c>
+      <c r="I1807" t="str">
+        <f t="shared" si="337"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1807" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1808" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1808" s="1">
+        <v>45412</v>
+      </c>
+      <c r="B1808" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1808" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1808">
+        <v>2.9</v>
+      </c>
+      <c r="E1808">
+        <f t="shared" si="333"/>
+        <v>4</v>
+      </c>
+      <c r="F1808">
+        <f t="shared" si="334"/>
+        <v>2024</v>
+      </c>
+      <c r="G1808">
+        <f t="shared" si="335"/>
+        <v>2</v>
+      </c>
+      <c r="H1808" t="str">
+        <f t="shared" si="336"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1808" t="str">
+        <f t="shared" si="337"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1808" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1809" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1809" s="1">
+        <v>45412</v>
+      </c>
+      <c r="B1809" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1809" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1809">
+        <v>0.79</v>
+      </c>
+      <c r="E1809">
+        <f t="shared" ref="E1809" si="338">MONTH(A1809)</f>
+        <v>4</v>
+      </c>
+      <c r="F1809">
+        <f t="shared" ref="F1809" si="339">YEAR(A1809)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1809">
+        <f t="shared" ref="G1809" si="340">WEEKDAY(A1809, 2)</f>
+        <v>2</v>
+      </c>
+      <c r="H1809" t="str">
+        <f t="shared" ref="H1809" si="341">CHOOSE(WEEKDAY(A1809, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1809" t="str">
+        <f t="shared" ref="I1809" si="342">TEXT(A1809, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1809" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1810" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1810" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1810" t="s">
+        <v>959</v>
+      </c>
+      <c r="C1810" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D1810">
+        <f>1.5/2</f>
+        <v>0.75</v>
+      </c>
+      <c r="E1810">
+        <f t="shared" ref="E1810" si="343">MONTH(A1810)</f>
+        <v>4</v>
+      </c>
+      <c r="F1810">
+        <f t="shared" ref="F1810" si="344">YEAR(A1810)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1810">
+        <f t="shared" ref="G1810" si="345">WEEKDAY(A1810, 2)</f>
+        <v>6</v>
+      </c>
+      <c r="H1810" t="str">
+        <f t="shared" ref="H1810" si="346">CHOOSE(WEEKDAY(A1810, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Saturday</v>
+      </c>
+      <c r="I1810" t="str">
+        <f t="shared" ref="I1810" si="347">TEXT(A1810, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1810" t="s">
+        <v>1020</v>
+      </c>
+      <c r="K1810" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="1811" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1811" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1811" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1811" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D1811">
+        <f>9.99/2</f>
+        <v>4.9950000000000001</v>
+      </c>
+      <c r="E1811">
+        <f t="shared" ref="E1811" si="348">MONTH(A1811)</f>
+        <v>4</v>
+      </c>
+      <c r="F1811">
+        <f t="shared" ref="F1811" si="349">YEAR(A1811)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1811">
+        <f t="shared" ref="G1811" si="350">WEEKDAY(A1811, 2)</f>
+        <v>6</v>
+      </c>
+      <c r="H1811" t="str">
+        <f t="shared" ref="H1811" si="351">CHOOSE(WEEKDAY(A1811, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Saturday</v>
+      </c>
+      <c r="I1811" t="str">
+        <f t="shared" ref="I1811" si="352">TEXT(A1811, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1811" t="s">
+        <v>1021</v>
+      </c>
+      <c r="K1811" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="1812" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1812" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1812" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1812" t="s">
+        <v>1023</v>
+      </c>
+      <c r="D1812">
+        <f>(7.99-7)/2</f>
+        <v>0.49500000000000011</v>
+      </c>
+      <c r="E1812">
+        <f t="shared" ref="E1812" si="353">MONTH(A1812)</f>
+        <v>4</v>
+      </c>
+      <c r="F1812">
+        <f t="shared" ref="F1812" si="354">YEAR(A1812)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1812">
+        <f t="shared" ref="G1812" si="355">WEEKDAY(A1812, 2)</f>
+        <v>6</v>
+      </c>
+      <c r="H1812" t="str">
+        <f t="shared" ref="H1812" si="356">CHOOSE(WEEKDAY(A1812, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Saturday</v>
+      </c>
+      <c r="I1812" t="str">
+        <f t="shared" ref="I1812" si="357">TEXT(A1812, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1812" t="s">
+        <v>1021</v>
+      </c>
+      <c r="K1812" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="1813" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1813" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1813" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1813" t="s">
+        <v>416</v>
+      </c>
+      <c r="D1813">
+        <v>2</v>
+      </c>
+      <c r="E1813">
+        <f t="shared" ref="E1813:E1814" si="358">MONTH(A1813)</f>
+        <v>4</v>
+      </c>
+      <c r="F1813">
+        <f t="shared" ref="F1813:F1814" si="359">YEAR(A1813)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1813">
+        <f t="shared" ref="G1813:G1814" si="360">WEEKDAY(A1813, 2)</f>
+        <v>6</v>
+      </c>
+      <c r="H1813" t="str">
+        <f t="shared" ref="H1813:H1814" si="361">CHOOSE(WEEKDAY(A1813, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Saturday</v>
+      </c>
+      <c r="I1813" t="str">
+        <f t="shared" ref="I1813:I1814" si="362">TEXT(A1813, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1813" t="s">
+        <v>1024</v>
+      </c>
+      <c r="K1813" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="1814" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1814" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1814" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1814" t="s">
+        <v>1025</v>
+      </c>
+      <c r="D1814">
+        <f>11/2</f>
+        <v>5.5</v>
+      </c>
+      <c r="E1814">
+        <f t="shared" si="358"/>
+        <v>4</v>
+      </c>
+      <c r="F1814">
+        <f t="shared" si="359"/>
+        <v>2024</v>
+      </c>
+      <c r="G1814">
+        <f t="shared" si="360"/>
+        <v>6</v>
+      </c>
+      <c r="H1814" t="str">
+        <f t="shared" si="361"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1814" t="str">
+        <f t="shared" si="362"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1814" t="s">
+        <v>1024</v>
+      </c>
+      <c r="K1814" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="1815" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1815" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1815" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1815" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D1815">
+        <f>1.5/2</f>
+        <v>0.75</v>
+      </c>
+      <c r="E1815">
+        <f t="shared" ref="E1815" si="363">MONTH(A1815)</f>
+        <v>4</v>
+      </c>
+      <c r="F1815">
+        <f t="shared" ref="F1815" si="364">YEAR(A1815)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1815">
+        <f t="shared" ref="G1815" si="365">WEEKDAY(A1815, 2)</f>
+        <v>6</v>
+      </c>
+      <c r="H1815" t="str">
+        <f t="shared" ref="H1815" si="366">CHOOSE(WEEKDAY(A1815, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Saturday</v>
+      </c>
+      <c r="I1815" t="str">
+        <f t="shared" ref="I1815" si="367">TEXT(A1815, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1815" t="s">
+        <v>1024</v>
+      </c>
+      <c r="K1815" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="1816" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1816" s="1">
+        <v>45409</v>
+      </c>
+      <c r="B1816" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1816" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D1816">
+        <v>1.3</v>
+      </c>
+      <c r="E1816">
+        <f t="shared" ref="E1816:E1817" si="368">MONTH(A1816)</f>
+        <v>4</v>
+      </c>
+      <c r="F1816">
+        <f t="shared" ref="F1816:F1817" si="369">YEAR(A1816)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1816">
+        <f t="shared" ref="G1816:G1817" si="370">WEEKDAY(A1816, 2)</f>
+        <v>6</v>
+      </c>
+      <c r="H1816" t="str">
+        <f t="shared" ref="H1816:H1817" si="371">CHOOSE(WEEKDAY(A1816, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Saturday</v>
+      </c>
+      <c r="I1816" t="str">
+        <f t="shared" ref="I1816:I1817" si="372">TEXT(A1816, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1816" t="s">
+        <v>1005</v>
+      </c>
+      <c r="K1816" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="1817" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1817" s="1">
+        <v>45412</v>
+      </c>
+      <c r="B1817" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1817" t="s">
+        <v>911</v>
+      </c>
+      <c r="D1817">
+        <f>2.89-0.7</f>
+        <v>2.1900000000000004</v>
+      </c>
+      <c r="E1817">
+        <f t="shared" si="368"/>
+        <v>4</v>
+      </c>
+      <c r="F1817">
+        <f t="shared" si="369"/>
+        <v>2024</v>
+      </c>
+      <c r="G1817">
+        <f t="shared" si="370"/>
+        <v>2</v>
+      </c>
+      <c r="H1817" t="str">
+        <f t="shared" si="371"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1817" t="str">
+        <f t="shared" si="372"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1817" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1817" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1818" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1818" s="1">
+        <v>45412</v>
+      </c>
+      <c r="B1818" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1818" t="s">
+        <v>911</v>
+      </c>
+      <c r="D1818">
+        <f>2.89-0.7</f>
+        <v>2.1900000000000004</v>
+      </c>
+      <c r="E1818">
+        <f t="shared" ref="E1818" si="373">MONTH(A1818)</f>
+        <v>4</v>
+      </c>
+      <c r="F1818">
+        <f t="shared" ref="F1818" si="374">YEAR(A1818)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1818">
+        <f t="shared" ref="G1818" si="375">WEEKDAY(A1818, 2)</f>
+        <v>2</v>
+      </c>
+      <c r="H1818" t="str">
+        <f t="shared" ref="H1818" si="376">CHOOSE(WEEKDAY(A1818, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1818" t="str">
+        <f t="shared" ref="I1818" si="377">TEXT(A1818, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1818" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1818" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1819" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1819" s="1">
+        <v>45412</v>
+      </c>
+      <c r="B1819" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1819" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D1819">
+        <v>0.99</v>
+      </c>
+      <c r="E1819">
+        <f t="shared" ref="E1819:E1824" si="378">MONTH(A1819)</f>
+        <v>4</v>
+      </c>
+      <c r="F1819">
+        <f t="shared" ref="F1819:F1824" si="379">YEAR(A1819)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1819">
+        <f t="shared" ref="G1819:G1824" si="380">WEEKDAY(A1819, 2)</f>
+        <v>2</v>
+      </c>
+      <c r="H1819" t="str">
+        <f t="shared" ref="H1819:H1824" si="381">CHOOSE(WEEKDAY(A1819, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1819" t="str">
+        <f t="shared" ref="I1819:I1824" si="382">TEXT(A1819, "MMM")</f>
+        <v>Apr</v>
+      </c>
+      <c r="J1819" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1819" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1820" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1820" s="1">
+        <v>45412</v>
+      </c>
+      <c r="B1820" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1820" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D1820">
+        <v>0.99</v>
+      </c>
+      <c r="E1820">
+        <f t="shared" si="378"/>
+        <v>4</v>
+      </c>
+      <c r="F1820">
+        <f t="shared" si="379"/>
+        <v>2024</v>
+      </c>
+      <c r="G1820">
+        <f t="shared" si="380"/>
+        <v>2</v>
+      </c>
+      <c r="H1820" t="str">
+        <f t="shared" si="381"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1820" t="str">
+        <f t="shared" si="382"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1820" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1820" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1821" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1821" s="1">
+        <v>45412</v>
+      </c>
+      <c r="B1821" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1821" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D1821">
+        <v>0.99</v>
+      </c>
+      <c r="E1821">
+        <f t="shared" si="378"/>
+        <v>4</v>
+      </c>
+      <c r="F1821">
+        <f t="shared" si="379"/>
+        <v>2024</v>
+      </c>
+      <c r="G1821">
+        <f t="shared" si="380"/>
+        <v>2</v>
+      </c>
+      <c r="H1821" t="str">
+        <f t="shared" si="381"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1821" t="str">
+        <f t="shared" si="382"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1821" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1821" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1822" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1822" s="1">
+        <v>45412</v>
+      </c>
+      <c r="B1822" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1822" t="s">
+        <v>1029</v>
+      </c>
+      <c r="D1822">
+        <v>1.19</v>
+      </c>
+      <c r="E1822">
+        <f t="shared" si="378"/>
+        <v>4</v>
+      </c>
+      <c r="F1822">
+        <f t="shared" si="379"/>
+        <v>2024</v>
+      </c>
+      <c r="G1822">
+        <f t="shared" si="380"/>
+        <v>2</v>
+      </c>
+      <c r="H1822" t="str">
+        <f t="shared" si="381"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1822" t="str">
+        <f t="shared" si="382"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1822" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1822" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1823" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1823" s="1">
+        <v>45412</v>
+      </c>
+      <c r="B1823" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1823" t="s">
+        <v>1029</v>
+      </c>
+      <c r="D1823">
+        <v>1.19</v>
+      </c>
+      <c r="E1823">
+        <f t="shared" si="378"/>
+        <v>4</v>
+      </c>
+      <c r="F1823">
+        <f t="shared" si="379"/>
+        <v>2024</v>
+      </c>
+      <c r="G1823">
+        <f t="shared" si="380"/>
+        <v>2</v>
+      </c>
+      <c r="H1823" t="str">
+        <f t="shared" si="381"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1823" t="str">
+        <f t="shared" si="382"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1823" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1823" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1824" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1824" s="1">
+        <v>45412</v>
+      </c>
+      <c r="B1824" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1824" t="s">
+        <v>1029</v>
+      </c>
+      <c r="D1824">
+        <v>1.19</v>
+      </c>
+      <c r="E1824">
+        <f t="shared" si="378"/>
+        <v>4</v>
+      </c>
+      <c r="F1824">
+        <f t="shared" si="379"/>
+        <v>2024</v>
+      </c>
+      <c r="G1824">
+        <f t="shared" si="380"/>
+        <v>2</v>
+      </c>
+      <c r="H1824" t="str">
+        <f t="shared" si="381"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1824" t="str">
+        <f t="shared" si="382"/>
+        <v>Apr</v>
+      </c>
+      <c r="J1824" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1824" t="s">
+        <v>730</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:L1803" xr:uid="{397426C9-9494-4E73-BF9B-2DE40DB1433B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E984">
     <sortCondition ref="A965:A984"/>
   </sortState>

</xml_diff>

<commit_message>
Add: add more expenses
</commit_message>
<xml_diff>
--- a/data/expense_tracker.xlsx
+++ b/data/expense_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\solutions\learning_python\expense_tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EDA535-3CE7-4F94-9A83-49CAEC66042B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49257D50-E4AB-4A03-B4FA-05C79BFBE8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" xr2:uid="{7A62D1F9-0105-4F41-8BB8-21CA3D721AF6}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6732" uniqueCount="1030">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6821" uniqueCount="1042">
   <si>
     <t>expense_type</t>
   </si>
@@ -3130,6 +3130,42 @@
   </si>
   <si>
     <t>best moments 85%</t>
+  </si>
+  <si>
+    <t>flying goose sriracha wasabi 200ml</t>
+  </si>
+  <si>
+    <t>pocky cookies &amp; cream 40g</t>
+  </si>
+  <si>
+    <t>modern asia market</t>
+  </si>
+  <si>
+    <t>basic kuchenrolle</t>
+  </si>
+  <si>
+    <t>vanillejog. Schokomuesli</t>
+  </si>
+  <si>
+    <t>protein pita roll chicken</t>
+  </si>
+  <si>
+    <t>franziskaner fi.</t>
+  </si>
+  <si>
+    <t>rm apfel rot tasse 0.797kgx1.99</t>
+  </si>
+  <si>
+    <t>apfel 0,998x1,89kg</t>
+  </si>
+  <si>
+    <t>spar curly-fries 600g</t>
+  </si>
+  <si>
+    <t>spar gitterpommes</t>
+  </si>
+  <si>
+    <t>spar highprotknm 500g</t>
   </si>
 </sst>
 </file>
@@ -3482,11 +3518,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397426C9-9494-4E73-BF9B-2DE40DB1433B}">
-  <dimension ref="A1:L1824"/>
+  <dimension ref="A1:L1848"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1801" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1810" sqref="I1810"/>
+      <pane ySplit="1" topLeftCell="A1826" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1835" sqref="H1835"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -70266,23 +70302,23 @@
         <v>0.99</v>
       </c>
       <c r="E1819">
-        <f t="shared" ref="E1819:E1824" si="378">MONTH(A1819)</f>
+        <f t="shared" ref="E1819:E1825" si="378">MONTH(A1819)</f>
         <v>4</v>
       </c>
       <c r="F1819">
-        <f t="shared" ref="F1819:F1824" si="379">YEAR(A1819)</f>
+        <f t="shared" ref="F1819:F1825" si="379">YEAR(A1819)</f>
         <v>2024</v>
       </c>
       <c r="G1819">
-        <f t="shared" ref="G1819:G1824" si="380">WEEKDAY(A1819, 2)</f>
+        <f t="shared" ref="G1819:G1825" si="380">WEEKDAY(A1819, 2)</f>
         <v>2</v>
       </c>
       <c r="H1819" t="str">
-        <f t="shared" ref="H1819:H1824" si="381">CHOOSE(WEEKDAY(A1819, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <f t="shared" ref="H1819:H1825" si="381">CHOOSE(WEEKDAY(A1819, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
         <v>Tuesday</v>
       </c>
       <c r="I1819" t="str">
-        <f t="shared" ref="I1819:I1824" si="382">TEXT(A1819, "MMM")</f>
+        <f t="shared" ref="I1819:I1825" si="382">TEXT(A1819, "MMM")</f>
         <v>Apr</v>
       </c>
       <c r="J1819" t="s">
@@ -70489,6 +70525,950 @@
         <v>47</v>
       </c>
       <c r="K1824" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1825" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1825" s="1">
+        <v>45414</v>
+      </c>
+      <c r="B1825" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1825" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1825">
+        <v>2.9</v>
+      </c>
+      <c r="E1825">
+        <f t="shared" si="378"/>
+        <v>5</v>
+      </c>
+      <c r="F1825">
+        <f t="shared" si="379"/>
+        <v>2024</v>
+      </c>
+      <c r="G1825">
+        <f t="shared" si="380"/>
+        <v>4</v>
+      </c>
+      <c r="H1825" t="str">
+        <f t="shared" si="381"/>
+        <v>Thursday</v>
+      </c>
+      <c r="I1825" t="str">
+        <f t="shared" si="382"/>
+        <v>May</v>
+      </c>
+      <c r="J1825" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1826" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1826" s="1">
+        <v>45414</v>
+      </c>
+      <c r="B1826" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1826" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1826">
+        <v>0.79</v>
+      </c>
+      <c r="E1826">
+        <f t="shared" ref="E1826:E1827" si="383">MONTH(A1826)</f>
+        <v>5</v>
+      </c>
+      <c r="F1826">
+        <f t="shared" ref="F1826:F1827" si="384">YEAR(A1826)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1826">
+        <f t="shared" ref="G1826:G1827" si="385">WEEKDAY(A1826, 2)</f>
+        <v>4</v>
+      </c>
+      <c r="H1826" t="str">
+        <f t="shared" ref="H1826:H1827" si="386">CHOOSE(WEEKDAY(A1826, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Thursday</v>
+      </c>
+      <c r="I1826" t="str">
+        <f t="shared" ref="I1826:I1827" si="387">TEXT(A1826, "MMM")</f>
+        <v>May</v>
+      </c>
+      <c r="J1826" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1827" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1827" s="1">
+        <v>45415</v>
+      </c>
+      <c r="B1827" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1827" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1827">
+        <v>3.3</v>
+      </c>
+      <c r="E1827">
+        <f t="shared" si="383"/>
+        <v>5</v>
+      </c>
+      <c r="F1827">
+        <f t="shared" si="384"/>
+        <v>2024</v>
+      </c>
+      <c r="G1827">
+        <f t="shared" si="385"/>
+        <v>5</v>
+      </c>
+      <c r="H1827" t="str">
+        <f t="shared" si="386"/>
+        <v>Friday</v>
+      </c>
+      <c r="I1827" t="str">
+        <f t="shared" si="387"/>
+        <v>May</v>
+      </c>
+      <c r="J1827" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1828" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1828" s="1">
+        <v>45415</v>
+      </c>
+      <c r="B1828" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1828" t="s">
+        <v>640</v>
+      </c>
+      <c r="D1828">
+        <v>0.79</v>
+      </c>
+      <c r="E1828">
+        <f t="shared" ref="E1828:E1829" si="388">MONTH(A1828)</f>
+        <v>5</v>
+      </c>
+      <c r="F1828">
+        <f t="shared" ref="F1828:F1829" si="389">YEAR(A1828)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1828">
+        <f t="shared" ref="G1828:G1829" si="390">WEEKDAY(A1828, 2)</f>
+        <v>5</v>
+      </c>
+      <c r="H1828" t="str">
+        <f t="shared" ref="H1828:H1829" si="391">CHOOSE(WEEKDAY(A1828, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Friday</v>
+      </c>
+      <c r="I1828" t="str">
+        <f t="shared" ref="I1828:I1829" si="392">TEXT(A1828, "MMM")</f>
+        <v>May</v>
+      </c>
+      <c r="J1828" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1829" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1829" s="1">
+        <v>45416</v>
+      </c>
+      <c r="B1829" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1829" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D1829">
+        <v>2.6</v>
+      </c>
+      <c r="E1829">
+        <f t="shared" si="388"/>
+        <v>5</v>
+      </c>
+      <c r="F1829">
+        <f t="shared" si="389"/>
+        <v>2024</v>
+      </c>
+      <c r="G1829">
+        <f t="shared" si="390"/>
+        <v>6</v>
+      </c>
+      <c r="H1829" t="str">
+        <f t="shared" si="391"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1829" t="str">
+        <f t="shared" si="392"/>
+        <v>May</v>
+      </c>
+      <c r="J1829" t="s">
+        <v>1032</v>
+      </c>
+      <c r="K1829" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="1830" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1830" s="1">
+        <v>45416</v>
+      </c>
+      <c r="B1830" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1830" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D1830">
+        <v>2.5</v>
+      </c>
+      <c r="E1830">
+        <f t="shared" ref="E1830" si="393">MONTH(A1830)</f>
+        <v>5</v>
+      </c>
+      <c r="F1830">
+        <f t="shared" ref="F1830" si="394">YEAR(A1830)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1830">
+        <f t="shared" ref="G1830" si="395">WEEKDAY(A1830, 2)</f>
+        <v>6</v>
+      </c>
+      <c r="H1830" t="str">
+        <f t="shared" ref="H1830" si="396">CHOOSE(WEEKDAY(A1830, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Saturday</v>
+      </c>
+      <c r="I1830" t="str">
+        <f t="shared" ref="I1830" si="397">TEXT(A1830, "MMM")</f>
+        <v>May</v>
+      </c>
+      <c r="J1830" t="s">
+        <v>1032</v>
+      </c>
+      <c r="K1830" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="1831" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1831" s="1">
+        <v>45416</v>
+      </c>
+      <c r="B1831" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1831" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D1831">
+        <f>2.39/2</f>
+        <v>1.1950000000000001</v>
+      </c>
+      <c r="E1831">
+        <f t="shared" ref="E1831:E1833" si="398">MONTH(A1831)</f>
+        <v>5</v>
+      </c>
+      <c r="F1831">
+        <f t="shared" ref="F1831:F1833" si="399">YEAR(A1831)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1831">
+        <f t="shared" ref="G1831:G1833" si="400">WEEKDAY(A1831, 2)</f>
+        <v>6</v>
+      </c>
+      <c r="H1831" t="str">
+        <f t="shared" ref="H1831:H1833" si="401">CHOOSE(WEEKDAY(A1831, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Saturday</v>
+      </c>
+      <c r="I1831" t="str">
+        <f t="shared" ref="I1831:I1833" si="402">TEXT(A1831, "MMM")</f>
+        <v>May</v>
+      </c>
+      <c r="J1831" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1831" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="1832" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1832" s="1">
+        <v>45416</v>
+      </c>
+      <c r="B1832" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1832" t="s">
+        <v>1034</v>
+      </c>
+      <c r="D1832">
+        <f>3.82-1.91</f>
+        <v>1.91</v>
+      </c>
+      <c r="E1832">
+        <f t="shared" si="398"/>
+        <v>5</v>
+      </c>
+      <c r="F1832">
+        <f t="shared" si="399"/>
+        <v>2024</v>
+      </c>
+      <c r="G1832">
+        <f t="shared" si="400"/>
+        <v>6</v>
+      </c>
+      <c r="H1832" t="str">
+        <f t="shared" si="401"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1832" t="str">
+        <f t="shared" si="402"/>
+        <v>May</v>
+      </c>
+      <c r="J1832" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1832" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="1833" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1833" s="1">
+        <v>45418</v>
+      </c>
+      <c r="B1833" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1833" t="s">
+        <v>938</v>
+      </c>
+      <c r="D1833">
+        <v>2.4</v>
+      </c>
+      <c r="E1833">
+        <f t="shared" si="398"/>
+        <v>5</v>
+      </c>
+      <c r="F1833">
+        <f t="shared" si="399"/>
+        <v>2024</v>
+      </c>
+      <c r="G1833">
+        <f t="shared" si="400"/>
+        <v>1</v>
+      </c>
+      <c r="H1833" t="str">
+        <f t="shared" si="401"/>
+        <v>Monday</v>
+      </c>
+      <c r="I1833" t="str">
+        <f t="shared" si="402"/>
+        <v>May</v>
+      </c>
+      <c r="J1833" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1834" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1834" s="1">
+        <v>45419</v>
+      </c>
+      <c r="B1834" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1834" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1834">
+        <v>4.16</v>
+      </c>
+      <c r="E1834">
+        <f t="shared" ref="E1834:E1836" si="403">MONTH(A1834)</f>
+        <v>5</v>
+      </c>
+      <c r="F1834">
+        <f t="shared" ref="F1834:F1836" si="404">YEAR(A1834)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1834">
+        <f t="shared" ref="G1834:G1836" si="405">WEEKDAY(A1834, 2)</f>
+        <v>2</v>
+      </c>
+      <c r="H1834" t="str">
+        <f t="shared" ref="H1834:H1836" si="406">CHOOSE(WEEKDAY(A1834, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1834" t="str">
+        <f t="shared" ref="I1834:I1836" si="407">TEXT(A1834, "MMM")</f>
+        <v>May</v>
+      </c>
+      <c r="J1834" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1835" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1835" s="1">
+        <v>45420</v>
+      </c>
+      <c r="B1835" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1835" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1835">
+        <v>2.9</v>
+      </c>
+      <c r="E1835">
+        <f t="shared" si="403"/>
+        <v>5</v>
+      </c>
+      <c r="F1835">
+        <f t="shared" si="404"/>
+        <v>2024</v>
+      </c>
+      <c r="G1835">
+        <f t="shared" si="405"/>
+        <v>3</v>
+      </c>
+      <c r="H1835" t="str">
+        <f t="shared" si="406"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="I1835" t="str">
+        <f t="shared" si="407"/>
+        <v>May</v>
+      </c>
+      <c r="J1835" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1836" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1836" s="1">
+        <v>45419</v>
+      </c>
+      <c r="B1836" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1836" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D1836">
+        <v>3.79</v>
+      </c>
+      <c r="E1836">
+        <f t="shared" si="403"/>
+        <v>5</v>
+      </c>
+      <c r="F1836">
+        <f t="shared" si="404"/>
+        <v>2024</v>
+      </c>
+      <c r="G1836">
+        <f t="shared" si="405"/>
+        <v>2</v>
+      </c>
+      <c r="H1836" t="str">
+        <f t="shared" si="406"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1836" t="str">
+        <f t="shared" si="407"/>
+        <v>May</v>
+      </c>
+      <c r="J1836" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1836" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="1837" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1837" s="1">
+        <v>45419</v>
+      </c>
+      <c r="B1837" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1837" t="s">
+        <v>509</v>
+      </c>
+      <c r="D1837">
+        <v>1.69</v>
+      </c>
+      <c r="E1837">
+        <f t="shared" ref="E1837:E1839" si="408">MONTH(A1837)</f>
+        <v>5</v>
+      </c>
+      <c r="F1837">
+        <f t="shared" ref="F1837:F1839" si="409">YEAR(A1837)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1837">
+        <f t="shared" ref="G1837:G1839" si="410">WEEKDAY(A1837, 2)</f>
+        <v>2</v>
+      </c>
+      <c r="H1837" t="str">
+        <f t="shared" ref="H1837:H1839" si="411">CHOOSE(WEEKDAY(A1837, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1837" t="str">
+        <f t="shared" ref="I1837:I1839" si="412">TEXT(A1837, "MMM")</f>
+        <v>May</v>
+      </c>
+      <c r="J1837" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1837" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="1838" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1838" s="1">
+        <v>45419</v>
+      </c>
+      <c r="B1838" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1838" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D1838">
+        <v>1.29</v>
+      </c>
+      <c r="E1838">
+        <f t="shared" si="408"/>
+        <v>5</v>
+      </c>
+      <c r="F1838">
+        <f t="shared" si="409"/>
+        <v>2024</v>
+      </c>
+      <c r="G1838">
+        <f t="shared" si="410"/>
+        <v>2</v>
+      </c>
+      <c r="H1838" t="str">
+        <f t="shared" si="411"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="I1838" t="str">
+        <f t="shared" si="412"/>
+        <v>May</v>
+      </c>
+      <c r="J1838" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1838" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="1839" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1839" s="1">
+        <v>45420</v>
+      </c>
+      <c r="B1839" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1839" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D1839">
+        <v>1.59</v>
+      </c>
+      <c r="E1839">
+        <f t="shared" si="408"/>
+        <v>5</v>
+      </c>
+      <c r="F1839">
+        <f t="shared" si="409"/>
+        <v>2024</v>
+      </c>
+      <c r="G1839">
+        <f t="shared" si="410"/>
+        <v>3</v>
+      </c>
+      <c r="H1839" t="str">
+        <f t="shared" si="411"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="I1839" t="str">
+        <f t="shared" si="412"/>
+        <v>May</v>
+      </c>
+      <c r="J1839" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1839" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="1840" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1840" s="1">
+        <v>45420</v>
+      </c>
+      <c r="B1840" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1840" t="s">
+        <v>509</v>
+      </c>
+      <c r="D1840">
+        <v>1.69</v>
+      </c>
+      <c r="E1840">
+        <f t="shared" ref="E1840:E1842" si="413">MONTH(A1840)</f>
+        <v>5</v>
+      </c>
+      <c r="F1840">
+        <f t="shared" ref="F1840:F1842" si="414">YEAR(A1840)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1840">
+        <f t="shared" ref="G1840:G1842" si="415">WEEKDAY(A1840, 2)</f>
+        <v>3</v>
+      </c>
+      <c r="H1840" t="str">
+        <f t="shared" ref="H1840:H1842" si="416">CHOOSE(WEEKDAY(A1840, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Wednesday</v>
+      </c>
+      <c r="I1840" t="str">
+        <f t="shared" ref="I1840:I1842" si="417">TEXT(A1840, "MMM")</f>
+        <v>May</v>
+      </c>
+      <c r="J1840" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1840" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="1841" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1841" s="1">
+        <v>45416</v>
+      </c>
+      <c r="B1841" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1841" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1841">
+        <f>49.33/2</f>
+        <v>24.664999999999999</v>
+      </c>
+      <c r="E1841">
+        <f t="shared" si="413"/>
+        <v>5</v>
+      </c>
+      <c r="F1841">
+        <f t="shared" si="414"/>
+        <v>2024</v>
+      </c>
+      <c r="G1841">
+        <f t="shared" si="415"/>
+        <v>6</v>
+      </c>
+      <c r="H1841" t="str">
+        <f t="shared" si="416"/>
+        <v>Saturday</v>
+      </c>
+      <c r="I1841" t="str">
+        <f t="shared" si="417"/>
+        <v>May</v>
+      </c>
+      <c r="J1841" t="s">
+        <v>864</v>
+      </c>
+      <c r="K1841" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1842" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1842" s="1">
+        <v>45418</v>
+      </c>
+      <c r="B1842" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1842" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D1842">
+        <v>1.89</v>
+      </c>
+      <c r="E1842">
+        <f t="shared" si="413"/>
+        <v>5</v>
+      </c>
+      <c r="F1842">
+        <f t="shared" si="414"/>
+        <v>2024</v>
+      </c>
+      <c r="G1842">
+        <f t="shared" si="415"/>
+        <v>1</v>
+      </c>
+      <c r="H1842" t="str">
+        <f t="shared" si="416"/>
+        <v>Monday</v>
+      </c>
+      <c r="I1842" t="str">
+        <f t="shared" si="417"/>
+        <v>May</v>
+      </c>
+      <c r="J1842" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1842" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1843" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1843" s="1">
+        <v>45418</v>
+      </c>
+      <c r="B1843" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1843" t="s">
+        <v>818</v>
+      </c>
+      <c r="D1843">
+        <v>0.99</v>
+      </c>
+      <c r="E1843">
+        <f t="shared" ref="E1843:E1845" si="418">MONTH(A1843)</f>
+        <v>5</v>
+      </c>
+      <c r="F1843">
+        <f t="shared" ref="F1843:F1845" si="419">YEAR(A1843)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1843">
+        <f t="shared" ref="G1843:G1845" si="420">WEEKDAY(A1843, 2)</f>
+        <v>1</v>
+      </c>
+      <c r="H1843" t="str">
+        <f t="shared" ref="H1843:H1845" si="421">CHOOSE(WEEKDAY(A1843, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Monday</v>
+      </c>
+      <c r="I1843" t="str">
+        <f t="shared" ref="I1843:I1845" si="422">TEXT(A1843, "MMM")</f>
+        <v>May</v>
+      </c>
+      <c r="J1843" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1843" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1844" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1844" s="1">
+        <v>45418</v>
+      </c>
+      <c r="B1844" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1844" t="s">
+        <v>604</v>
+      </c>
+      <c r="D1844">
+        <v>0.99</v>
+      </c>
+      <c r="E1844">
+        <f t="shared" si="418"/>
+        <v>5</v>
+      </c>
+      <c r="F1844">
+        <f t="shared" si="419"/>
+        <v>2024</v>
+      </c>
+      <c r="G1844">
+        <f t="shared" si="420"/>
+        <v>1</v>
+      </c>
+      <c r="H1844" t="str">
+        <f t="shared" si="421"/>
+        <v>Monday</v>
+      </c>
+      <c r="I1844" t="str">
+        <f t="shared" si="422"/>
+        <v>May</v>
+      </c>
+      <c r="J1844" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1844" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1845" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1845" s="1">
+        <v>45420</v>
+      </c>
+      <c r="B1845" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1845" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D1845">
+        <f>(2.99-1)/2</f>
+        <v>0.99500000000000011</v>
+      </c>
+      <c r="E1845">
+        <f t="shared" si="418"/>
+        <v>5</v>
+      </c>
+      <c r="F1845">
+        <f t="shared" si="419"/>
+        <v>2024</v>
+      </c>
+      <c r="G1845">
+        <f t="shared" si="420"/>
+        <v>3</v>
+      </c>
+      <c r="H1845" t="str">
+        <f t="shared" si="421"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="I1845" t="str">
+        <f t="shared" si="422"/>
+        <v>May</v>
+      </c>
+      <c r="J1845" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1845" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1846" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1846" s="1">
+        <v>45420</v>
+      </c>
+      <c r="B1846" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1846" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D1846">
+        <f>(2.99-1)/2</f>
+        <v>0.99500000000000011</v>
+      </c>
+      <c r="E1846">
+        <f t="shared" ref="E1846" si="423">MONTH(A1846)</f>
+        <v>5</v>
+      </c>
+      <c r="F1846">
+        <f t="shared" ref="F1846" si="424">YEAR(A1846)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1846">
+        <f t="shared" ref="G1846" si="425">WEEKDAY(A1846, 2)</f>
+        <v>3</v>
+      </c>
+      <c r="H1846" t="str">
+        <f t="shared" ref="H1846" si="426">CHOOSE(WEEKDAY(A1846, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Wednesday</v>
+      </c>
+      <c r="I1846" t="str">
+        <f t="shared" ref="I1846" si="427">TEXT(A1846, "MMM")</f>
+        <v>May</v>
+      </c>
+      <c r="J1846" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1846" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1847" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1847" s="1">
+        <v>45420</v>
+      </c>
+      <c r="B1847" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1847" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1847">
+        <v>1.99</v>
+      </c>
+      <c r="E1847">
+        <f t="shared" ref="E1847" si="428">MONTH(A1847)</f>
+        <v>5</v>
+      </c>
+      <c r="F1847">
+        <f t="shared" ref="F1847" si="429">YEAR(A1847)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1847">
+        <f t="shared" ref="G1847" si="430">WEEKDAY(A1847, 2)</f>
+        <v>3</v>
+      </c>
+      <c r="H1847" t="str">
+        <f t="shared" ref="H1847" si="431">CHOOSE(WEEKDAY(A1847, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Wednesday</v>
+      </c>
+      <c r="I1847" t="str">
+        <f t="shared" ref="I1847" si="432">TEXT(A1847, "MMM")</f>
+        <v>May</v>
+      </c>
+      <c r="J1847" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1847" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="1848" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1848" s="1">
+        <v>45420</v>
+      </c>
+      <c r="B1848" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1848" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D1848">
+        <v>3.19</v>
+      </c>
+      <c r="E1848">
+        <f t="shared" ref="E1848" si="433">MONTH(A1848)</f>
+        <v>5</v>
+      </c>
+      <c r="F1848">
+        <f t="shared" ref="F1848" si="434">YEAR(A1848)</f>
+        <v>2024</v>
+      </c>
+      <c r="G1848">
+        <f t="shared" ref="G1848" si="435">WEEKDAY(A1848, 2)</f>
+        <v>3</v>
+      </c>
+      <c r="H1848" t="str">
+        <f t="shared" ref="H1848" si="436">CHOOSE(WEEKDAY(A1848, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Wednesday</v>
+      </c>
+      <c r="I1848" t="str">
+        <f t="shared" ref="I1848" si="437">TEXT(A1848, "MMM")</f>
+        <v>May</v>
+      </c>
+      <c r="J1848" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1848" t="s">
         <v>730</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add: add gas expenses
</commit_message>
<xml_diff>
--- a/data/expense_tracker.xlsx
+++ b/data/expense_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\solutions\learning_python\expense_tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFB028B-31E0-4099-8ECA-B8D04AECDC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCC8FB9-0FBA-4B67-9734-6251217DC365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" xr2:uid="{7A62D1F9-0105-4F41-8BB8-21CA3D721AF6}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6896" uniqueCount="1050">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6900" uniqueCount="1051">
   <si>
     <t>expense_type</t>
   </si>
@@ -3189,6 +3189,9 @@
   </si>
   <si>
     <t>apfel evelina (0,902kgx2.49eur/kg)</t>
+  </si>
+  <si>
+    <t>discont</t>
   </si>
 </sst>
 </file>
@@ -3542,11 +3545,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397426C9-9494-4E73-BF9B-2DE40DB1433B}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:L1875"/>
+  <dimension ref="A1:L1876"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1855" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1870" sqref="I1870"/>
+      <selection pane="bottomLeft" activeCell="A1877" sqref="A1877"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -76978,23 +76981,23 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="E1873">
-        <f t="shared" ref="E1873:E1875" si="191">MONTH(A1873)</f>
+        <f t="shared" ref="E1873:E1876" si="191">MONTH(A1873)</f>
         <v>5</v>
       </c>
       <c r="F1873">
-        <f t="shared" ref="F1873:F1875" si="192">YEAR(A1873)</f>
+        <f t="shared" ref="F1873:F1876" si="192">YEAR(A1873)</f>
         <v>2024</v>
       </c>
       <c r="G1873">
-        <f t="shared" ref="G1873:G1875" si="193">WEEKDAY(A1873, 2)</f>
+        <f t="shared" ref="G1873:G1876" si="193">WEEKDAY(A1873, 2)</f>
         <v>5</v>
       </c>
       <c r="H1873" t="str">
-        <f t="shared" ref="H1873:H1875" si="194">CHOOSE(WEEKDAY(A1873, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <f t="shared" ref="H1873:H1876" si="194">CHOOSE(WEEKDAY(A1873, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
         <v>Friday</v>
       </c>
       <c r="I1873" t="str">
-        <f t="shared" ref="I1873:I1875" si="195">TEXT(A1873, "MMM")</f>
+        <f t="shared" ref="I1873:I1876" si="195">TEXT(A1873, "MMM")</f>
         <v>May</v>
       </c>
       <c r="J1873" t="s">
@@ -77082,6 +77085,46 @@
         <v>49</v>
       </c>
       <c r="K1875" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="1876" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1876" s="1">
+        <v>45431</v>
+      </c>
+      <c r="B1876" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1876" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1876">
+        <v>27</v>
+      </c>
+      <c r="E1876">
+        <f t="shared" si="191"/>
+        <v>5</v>
+      </c>
+      <c r="F1876">
+        <f t="shared" si="192"/>
+        <v>2024</v>
+      </c>
+      <c r="G1876">
+        <f t="shared" si="193"/>
+        <v>7</v>
+      </c>
+      <c r="H1876" t="str">
+        <f t="shared" si="194"/>
+        <v>Sunday</v>
+      </c>
+      <c r="I1876" t="str">
+        <f t="shared" si="195"/>
+        <v>May</v>
+      </c>
+      <c r="J1876" t="s">
+        <v>1050</v>
+      </c>
+      <c r="K1876" t="s">
         <v>743</v>
       </c>
     </row>

</xml_diff>